<commit_message>
Finalize budget outputs under service level constraint
</commit_message>
<xml_diff>
--- a/Outputs/5. Budget constrained/Grid Search/Output Files/1500000/Output_10_2.xlsx
+++ b/Outputs/5. Budget constrained/Grid Search/Output Files/1500000/Output_10_2.xlsx
@@ -471,7 +471,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="4">
@@ -501,7 +501,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-2352871.676757053</v>
+        <v>-2355725.610014079</v>
       </c>
     </row>
     <row r="7">
@@ -521,7 +521,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>603248.4937673431</v>
+        <v>603248.493767343</v>
       </c>
     </row>
     <row r="9">
@@ -665,16 +665,16 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>189.1240288902036</v>
+        <v>95.74111878851791</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>406.8760457417114</v>
       </c>
       <c r="G2" t="n">
         <v>413.3734762915973</v>
       </c>
       <c r="H2" t="n">
-        <v>19.64416180581867</v>
+        <v>319.7167556102116</v>
       </c>
       <c r="I2" t="n">
         <v>136.0980462499685</v>
@@ -722,10 +722,10 @@
         <v>0</v>
       </c>
       <c r="X2" t="n">
-        <v>369.731100678469</v>
+        <v>0</v>
       </c>
       <c r="Y2" t="n">
-        <v>386.2379386560536</v>
+        <v>142.4033098901038</v>
       </c>
     </row>
     <row r="3">
@@ -747,7 +747,7 @@
         <v>157.6450804554009</v>
       </c>
       <c r="F3" t="n">
-        <v>145.0692123933839</v>
+        <v>113.3493063277841</v>
       </c>
       <c r="G3" t="n">
         <v>136.3112714057301</v>
@@ -756,7 +756,7 @@
         <v>102.2661233681972</v>
       </c>
       <c r="I3" t="n">
-        <v>22.13668645150612</v>
+        <v>53.85659251710582</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
@@ -817,7 +817,7 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>167.2468210986278</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
         <v>148.6154730182124</v>
@@ -868,16 +868,16 @@
         <v>0</v>
       </c>
       <c r="T4" t="n">
-        <v>0</v>
+        <v>224.2479705299724</v>
       </c>
       <c r="U4" t="n">
-        <v>0</v>
+        <v>286.2718257109806</v>
       </c>
       <c r="V4" t="n">
-        <v>252.137643323828</v>
+        <v>0</v>
       </c>
       <c r="W4" t="n">
-        <v>105.1362589376935</v>
+        <v>14.00092711919598</v>
       </c>
       <c r="X4" t="n">
         <v>0</v>
@@ -905,10 +905,10 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>6.876045741711437</v>
+        <v>406.8760457417114</v>
       </c>
       <c r="G5" t="n">
-        <v>12.9169039459368</v>
+        <v>412.9169039459368</v>
       </c>
       <c r="H5" t="n">
         <v>315.0408840752156</v>
@@ -944,25 +944,25 @@
         <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>154.6528871281402</v>
+        <v>0</v>
       </c>
       <c r="T5" t="n">
-        <v>212.651863114966</v>
+        <v>0</v>
       </c>
       <c r="U5" t="n">
-        <v>251.1547862223006</v>
+        <v>227.432740305242</v>
       </c>
       <c r="V5" t="n">
-        <v>0</v>
+        <v>327.7522584701349</v>
       </c>
       <c r="W5" t="n">
         <v>0</v>
       </c>
       <c r="X5" t="n">
-        <v>350.4875236539169</v>
+        <v>0</v>
       </c>
       <c r="Y5" t="n">
-        <v>386.2379386560536</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -1060,10 +1060,10 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>146.4339626465692</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>79.13107494872602</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -1075,7 +1075,7 @@
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>17.69584188176898</v>
+        <v>0</v>
       </c>
       <c r="K7" t="n">
         <v>0</v>
@@ -1108,10 +1108,10 @@
         <v>0</v>
       </c>
       <c r="U7" t="n">
-        <v>241.4221856852594</v>
+        <v>0</v>
       </c>
       <c r="V7" t="n">
-        <v>0</v>
+        <v>252.137643323828</v>
       </c>
       <c r="W7" t="n">
         <v>286.522998336591</v>
@@ -1120,7 +1120,7 @@
         <v>225.7096553890372</v>
       </c>
       <c r="Y7" t="n">
-        <v>218.5846533520948</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -1130,28 +1130,28 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>382.7338416634806</v>
       </c>
       <c r="C8" t="n">
         <v>365.2728917710076</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>354.683041620683</v>
       </c>
       <c r="E8" t="n">
-        <v>381.9303700722618</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
         <v>6.876045741711437</v>
       </c>
       <c r="G8" t="n">
-        <v>12.9169039459368</v>
+        <v>412.9169039459368</v>
       </c>
       <c r="H8" t="n">
-        <v>143.9112656986653</v>
+        <v>46.89975697558092</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>118.4960408938903</v>
       </c>
       <c r="J8" t="n">
         <v>0</v>
@@ -1181,10 +1181,10 @@
         <v>0</v>
       </c>
       <c r="S8" t="n">
-        <v>0</v>
+        <v>154.6528871281402</v>
       </c>
       <c r="T8" t="n">
-        <v>212.651863114966</v>
+        <v>0</v>
       </c>
       <c r="U8" t="n">
         <v>0</v>
@@ -1193,10 +1193,10 @@
         <v>327.7522584701349</v>
       </c>
       <c r="W8" t="n">
-        <v>349.240968717413</v>
+        <v>0</v>
       </c>
       <c r="X8" t="n">
-        <v>369.731100678469</v>
+        <v>0</v>
       </c>
       <c r="Y8" t="n">
         <v>386.2379386560536</v>
@@ -1288,7 +1288,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>179.8319801819373</v>
+        <v>0</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
@@ -1300,19 +1300,19 @@
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>52.71114119546518</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>166.9207765545704</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>152.7120966692326</v>
       </c>
       <c r="I10" t="n">
         <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>17.69584188176898</v>
       </c>
       <c r="K10" t="n">
         <v>0</v>
@@ -1339,7 +1339,7 @@
         <v>129.1731816677913</v>
       </c>
       <c r="S10" t="n">
-        <v>203.0828740821575</v>
+        <v>0</v>
       </c>
       <c r="T10" t="n">
         <v>0</v>
@@ -1354,10 +1354,10 @@
         <v>0</v>
       </c>
       <c r="X10" t="n">
-        <v>225.7096553890372</v>
+        <v>0</v>
       </c>
       <c r="Y10" t="n">
-        <v>0</v>
+        <v>218.5846533520948</v>
       </c>
     </row>
     <row r="11">
@@ -1424,10 +1424,10 @@
         <v>199.0222304576161</v>
       </c>
       <c r="U11" t="n">
-        <v>250.9057009881286</v>
+        <v>250.9057009881284</v>
       </c>
       <c r="V11" t="n">
-        <v>327.7522584701337</v>
+        <v>327.7522584701349</v>
       </c>
       <c r="W11" t="n">
         <v>349.240968717413</v>
@@ -1531,7 +1531,7 @@
         <v>167.2468210986278</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>148.6154730182124</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -1540,7 +1540,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>27.02919805176115</v>
+        <v>0</v>
       </c>
       <c r="H13" t="n">
         <v>140.2947128462239</v>
@@ -1588,7 +1588,7 @@
         <v>252.137643323828</v>
       </c>
       <c r="W13" t="n">
-        <v>286.522998336591</v>
+        <v>164.9367233701398</v>
       </c>
       <c r="X13" t="n">
         <v>225.7096553890372</v>
@@ -1661,7 +1661,7 @@
         <v>199.0222304576161</v>
       </c>
       <c r="U14" t="n">
-        <v>250.9057009881284</v>
+        <v>250.9057009881286</v>
       </c>
       <c r="V14" t="n">
         <v>327.7522584701349</v>
@@ -1768,10 +1768,10 @@
         <v>167.2468210986278</v>
       </c>
       <c r="D16" t="n">
-        <v>148.6154730182124</v>
+        <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>146.4339626465692</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -1813,10 +1813,10 @@
         <v>66.37524671012169</v>
       </c>
       <c r="S16" t="n">
-        <v>0</v>
+        <v>181.0262860016446</v>
       </c>
       <c r="T16" t="n">
-        <v>217.4054503272883</v>
+        <v>78.9105100867805</v>
       </c>
       <c r="U16" t="n">
         <v>286.1844743892441</v>
@@ -1828,10 +1828,10 @@
         <v>286.522998336591</v>
       </c>
       <c r="X16" t="n">
-        <v>191.7762188374877</v>
+        <v>225.7096553890372</v>
       </c>
       <c r="Y16" t="n">
-        <v>0</v>
+        <v>218.5846533520948</v>
       </c>
     </row>
     <row r="17">
@@ -1856,7 +1856,7 @@
         <v>406.8760457417114</v>
       </c>
       <c r="G17" t="n">
-        <v>409.8033385187852</v>
+        <v>409.8033385187866</v>
       </c>
       <c r="H17" t="n">
         <v>283.1540821444137</v>
@@ -2011,16 +2011,16 @@
         <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>145.4210480229312</v>
+        <v>0</v>
       </c>
       <c r="G19" t="n">
         <v>165.5241382922688</v>
       </c>
       <c r="H19" t="n">
-        <v>0</v>
+        <v>140.2947128462239</v>
       </c>
       <c r="I19" t="n">
-        <v>4.019807611472036</v>
+        <v>0</v>
       </c>
       <c r="J19" t="n">
         <v>0</v>
@@ -2047,7 +2047,7 @@
         <v>0</v>
       </c>
       <c r="R19" t="n">
-        <v>0</v>
+        <v>66.37524671012169</v>
       </c>
       <c r="S19" t="n">
         <v>181.0262860016446</v>
@@ -2062,7 +2062,7 @@
         <v>252.137643323828</v>
       </c>
       <c r="W19" t="n">
-        <v>286.522998336591</v>
+        <v>229.2938944146487</v>
       </c>
       <c r="X19" t="n">
         <v>225.7096553890372</v>
@@ -2129,7 +2129,7 @@
         <v>0</v>
       </c>
       <c r="S20" t="n">
-        <v>83.70251495695439</v>
+        <v>83.70251495695528</v>
       </c>
       <c r="T20" t="n">
         <v>199.0222304576161</v>
@@ -2333,7 +2333,7 @@
         <v>409.8033385187866</v>
       </c>
       <c r="H23" t="n">
-        <v>283.1540821444137</v>
+        <v>283.1540821444132</v>
       </c>
       <c r="I23" t="n">
         <v>0</v>
@@ -2372,7 +2372,7 @@
         <v>199.0222304576161</v>
       </c>
       <c r="U23" t="n">
-        <v>250.9057009881275</v>
+        <v>250.9057009881286</v>
       </c>
       <c r="V23" t="n">
         <v>327.7522584701349</v>
@@ -2482,16 +2482,16 @@
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>146.4339626465692</v>
+        <v>0</v>
       </c>
       <c r="F25" t="n">
         <v>0</v>
       </c>
       <c r="G25" t="n">
-        <v>102.1557845699813</v>
+        <v>108.2950343703266</v>
       </c>
       <c r="H25" t="n">
-        <v>0</v>
+        <v>140.2947128462239</v>
       </c>
       <c r="I25" t="n">
         <v>0</v>
@@ -2552,7 +2552,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>382.7338416634806</v>
+        <v>382.7338416634794</v>
       </c>
       <c r="C26" t="n">
         <v>365.2728917710076</v>
@@ -2564,7 +2564,7 @@
         <v>381.9303700722618</v>
       </c>
       <c r="F26" t="n">
-        <v>406.8760457417101</v>
+        <v>406.8760457417114</v>
       </c>
       <c r="G26" t="n">
         <v>409.8033385187866</v>
@@ -2719,10 +2719,10 @@
         <v>124.3308255261726</v>
       </c>
       <c r="E28" t="n">
-        <v>122.1493151545294</v>
+        <v>122.1493151545303</v>
       </c>
       <c r="F28" t="n">
-        <v>121.1364005308922</v>
+        <v>121.1364005308915</v>
       </c>
       <c r="G28" t="n">
         <v>141.2394908002291</v>
@@ -2953,13 +2953,13 @@
         <v>142.9621736065881</v>
       </c>
       <c r="D31" t="n">
-        <v>124.3308255261726</v>
+        <v>124.3308255261734</v>
       </c>
       <c r="E31" t="n">
         <v>122.1493151545294</v>
       </c>
       <c r="F31" t="n">
-        <v>121.1364005308922</v>
+        <v>121.1364005308915</v>
       </c>
       <c r="G31" t="n">
         <v>141.2394908002291</v>
@@ -3041,7 +3041,7 @@
         <v>406.8760457417114</v>
       </c>
       <c r="G32" t="n">
-        <v>409.8033385187852</v>
+        <v>409.8033385187866</v>
       </c>
       <c r="H32" t="n">
         <v>283.1540821444137</v>
@@ -3080,7 +3080,7 @@
         <v>83.7025149569553</v>
       </c>
       <c r="T32" t="n">
-        <v>199.0222304576161</v>
+        <v>199.0222304576164</v>
       </c>
       <c r="U32" t="n">
         <v>250.9057009881286</v>
@@ -3232,7 +3232,7 @@
         <v>0</v>
       </c>
       <c r="R34" t="n">
-        <v>42.09059921808195</v>
+        <v>42.09059921808194</v>
       </c>
       <c r="S34" t="n">
         <v>156.7416385096049</v>
@@ -3272,7 +3272,7 @@
         <v>354.683041620683</v>
       </c>
       <c r="E35" t="n">
-        <v>381.9303700722614</v>
+        <v>381.9303700722618</v>
       </c>
       <c r="F35" t="n">
         <v>406.8760457417114</v>
@@ -3320,7 +3320,7 @@
         <v>199.0222304576161</v>
       </c>
       <c r="U35" t="n">
-        <v>250.9057009881286</v>
+        <v>250.9057009881275</v>
       </c>
       <c r="V35" t="n">
         <v>327.7522584701349</v>
@@ -3430,7 +3430,7 @@
         <v>124.3308255261726</v>
       </c>
       <c r="E37" t="n">
-        <v>122.1493151545294</v>
+        <v>122.1493151545295</v>
       </c>
       <c r="F37" t="n">
         <v>121.1364005308915</v>
@@ -3439,10 +3439,10 @@
         <v>141.2394908002291</v>
       </c>
       <c r="H37" t="n">
-        <v>116.0100653541841</v>
+        <v>116.0100653541842</v>
       </c>
       <c r="I37" t="n">
-        <v>56.98118882652579</v>
+        <v>56.98118882652582</v>
       </c>
       <c r="J37" t="n">
         <v>0</v>
@@ -3469,13 +3469,13 @@
         <v>0</v>
       </c>
       <c r="R37" t="n">
-        <v>42.09059921808195</v>
+        <v>42.09059921808198</v>
       </c>
       <c r="S37" t="n">
         <v>156.7416385096049</v>
       </c>
       <c r="T37" t="n">
-        <v>193.1208028352485</v>
+        <v>193.1208028352486</v>
       </c>
       <c r="U37" t="n">
         <v>261.8998268972044</v>
@@ -3500,7 +3500,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>382.7338416634803</v>
+        <v>382.7338416634806</v>
       </c>
       <c r="C38" t="n">
         <v>365.2728917710076</v>
@@ -3661,25 +3661,25 @@
         <v>155.5473326898976</v>
       </c>
       <c r="C40" t="n">
-        <v>142.9621736065882</v>
+        <v>142.9621736065881</v>
       </c>
       <c r="D40" t="n">
-        <v>124.3308255261727</v>
+        <v>124.3308255261726</v>
       </c>
       <c r="E40" t="n">
-        <v>122.1493151545295</v>
+        <v>122.1493151545294</v>
       </c>
       <c r="F40" t="n">
-        <v>121.1364005308916</v>
+        <v>121.1364005308915</v>
       </c>
       <c r="G40" t="n">
-        <v>141.2394908002292</v>
+        <v>141.2394908002291</v>
       </c>
       <c r="H40" t="n">
-        <v>116.0100653541842</v>
+        <v>116.0100653541841</v>
       </c>
       <c r="I40" t="n">
-        <v>56.98118882652585</v>
+        <v>56.98118882652579</v>
       </c>
       <c r="J40" t="n">
         <v>0</v>
@@ -3706,13 +3706,13 @@
         <v>0</v>
       </c>
       <c r="R40" t="n">
-        <v>42.090599218082</v>
+        <v>42.09059921808195</v>
       </c>
       <c r="S40" t="n">
         <v>156.7416385096049</v>
       </c>
       <c r="T40" t="n">
-        <v>193.1208028352486</v>
+        <v>193.1208028352485</v>
       </c>
       <c r="U40" t="n">
         <v>261.8998268972044</v>
@@ -3724,7 +3724,7 @@
         <v>262.2383508445513</v>
       </c>
       <c r="X40" t="n">
-        <v>201.4250078969975</v>
+        <v>201.4250078969974</v>
       </c>
       <c r="Y40" t="n">
         <v>194.3000058600551</v>
@@ -3913,10 +3913,10 @@
         <v>141.2394908002291</v>
       </c>
       <c r="H43" t="n">
-        <v>116.0100653541841</v>
+        <v>116.0100653541842</v>
       </c>
       <c r="I43" t="n">
-        <v>56.9811888265258</v>
+        <v>56.98118882652581</v>
       </c>
       <c r="J43" t="n">
         <v>0</v>
@@ -3977,7 +3977,7 @@
         <v>382.7338416634806</v>
       </c>
       <c r="C44" t="n">
-        <v>365.2728917710076</v>
+        <v>365.2728917710071</v>
       </c>
       <c r="D44" t="n">
         <v>354.683041620683</v>
@@ -4304,22 +4304,22 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>818.599619779601</v>
+        <v>1438.362982854771</v>
       </c>
       <c r="C2" t="n">
-        <v>818.599619779601</v>
+        <v>1438.362982854771</v>
       </c>
       <c r="D2" t="n">
-        <v>818.599619779601</v>
+        <v>1438.362982854771</v>
       </c>
       <c r="E2" t="n">
-        <v>627.5652471632337</v>
+        <v>1341.654782058289</v>
       </c>
       <c r="F2" t="n">
-        <v>627.5652471632337</v>
+        <v>930.6688772686811</v>
       </c>
       <c r="G2" t="n">
-        <v>210.0162812121252</v>
+        <v>513.1199113175726</v>
       </c>
       <c r="H2" t="n">
         <v>190.1736935294801</v>
@@ -4328,25 +4328,25 @@
         <v>52.70091953961285</v>
       </c>
       <c r="J2" t="n">
-        <v>202.9773215020674</v>
+        <v>52.70091953961285</v>
       </c>
       <c r="K2" t="n">
-        <v>228.0435387074851</v>
+        <v>398.6710951904836</v>
       </c>
       <c r="L2" t="n">
-        <v>709.5267619202357</v>
+        <v>880.1543184032342</v>
       </c>
       <c r="M2" t="n">
-        <v>1261.87616510248</v>
+        <v>1432.503721585478</v>
       </c>
       <c r="N2" t="n">
-        <v>1808.531161545922</v>
+        <v>1979.15871802892</v>
       </c>
       <c r="O2" t="n">
-        <v>2074.365717271178</v>
+        <v>2450.161892029133</v>
       </c>
       <c r="P2" t="n">
-        <v>2438.681646329268</v>
+        <v>2635.045976980643</v>
       </c>
       <c r="Q2" t="n">
         <v>2635.045976980643</v>
@@ -4370,10 +4370,10 @@
         <v>1968.804550080614</v>
       </c>
       <c r="X2" t="n">
-        <v>1595.338791819534</v>
+        <v>1968.804550080614</v>
       </c>
       <c r="Y2" t="n">
-        <v>1205.199459843723</v>
+        <v>1824.962822918893</v>
       </c>
     </row>
     <row r="3">
@@ -4395,37 +4395,37 @@
         <v>462.5830343060949</v>
       </c>
       <c r="F3" t="n">
-        <v>316.0484763329799</v>
+        <v>348.0887854901514</v>
       </c>
       <c r="G3" t="n">
-        <v>178.3603233978991</v>
+        <v>210.4006325550705</v>
       </c>
       <c r="H3" t="n">
-        <v>75.06120888456853</v>
+        <v>107.10151804174</v>
       </c>
       <c r="I3" t="n">
         <v>52.70091953961285</v>
       </c>
       <c r="J3" t="n">
-        <v>148.5111353690306</v>
+        <v>52.70091953961285</v>
       </c>
       <c r="K3" t="n">
-        <v>438.8868977629675</v>
+        <v>81.25609729109699</v>
       </c>
       <c r="L3" t="n">
-        <v>890.737341183225</v>
+        <v>533.1065407113545</v>
       </c>
       <c r="M3" t="n">
-        <v>1470.004717886419</v>
+        <v>1112.373917414548</v>
       </c>
       <c r="N3" t="n">
-        <v>2080.310591774529</v>
+        <v>1722.679791302658</v>
       </c>
       <c r="O3" t="n">
-        <v>2572.205555200545</v>
+        <v>2214.574754728675</v>
       </c>
       <c r="P3" t="n">
-        <v>2635.045976980643</v>
+        <v>2592.360761426663</v>
       </c>
       <c r="Q3" t="n">
         <v>2635.045976980643</v>
@@ -4462,7 +4462,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2274.16324742355</v>
+        <v>2105.227064495643</v>
       </c>
       <c r="C4" t="n">
         <v>2105.227064495643</v>
@@ -4516,22 +4516,22 @@
         <v>2635.045976980643</v>
       </c>
       <c r="T4" t="n">
-        <v>2635.045976980643</v>
+        <v>2408.532875435216</v>
       </c>
       <c r="U4" t="n">
-        <v>2635.045976980643</v>
+        <v>2119.369415121094</v>
       </c>
       <c r="V4" t="n">
-        <v>2380.361488774756</v>
+        <v>2119.369415121094</v>
       </c>
       <c r="W4" t="n">
-        <v>2274.16324742355</v>
+        <v>2105.227064495643</v>
       </c>
       <c r="X4" t="n">
-        <v>2274.16324742355</v>
+        <v>2105.227064495643</v>
       </c>
       <c r="Y4" t="n">
-        <v>2274.16324742355</v>
+        <v>2105.227064495643</v>
       </c>
     </row>
     <row r="5">
@@ -4541,19 +4541,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>879.5724007797762</v>
+        <v>1687.653208860584</v>
       </c>
       <c r="C5" t="n">
-        <v>510.6098838393645</v>
+        <v>1318.690691920173</v>
       </c>
       <c r="D5" t="n">
-        <v>510.6098838393645</v>
+        <v>1318.690691920173</v>
       </c>
       <c r="E5" t="n">
-        <v>510.6098838393645</v>
+        <v>1318.690691920173</v>
       </c>
       <c r="F5" t="n">
-        <v>503.664383090161</v>
+        <v>907.7047871305651</v>
       </c>
       <c r="G5" t="n">
         <v>490.6170053669925</v>
@@ -4568,19 +4568,19 @@
         <v>73.93516953299616</v>
       </c>
       <c r="K5" t="n">
-        <v>225.231470968264</v>
+        <v>156.4983241075885</v>
       </c>
       <c r="L5" t="n">
-        <v>364.5601268095172</v>
+        <v>709.3115823537878</v>
       </c>
       <c r="M5" t="n">
-        <v>996.277937792829</v>
+        <v>1341.029393337099</v>
       </c>
       <c r="N5" t="n">
-        <v>1623.585605852676</v>
+        <v>1968.337061396946</v>
       </c>
       <c r="O5" t="n">
-        <v>2170.746810619753</v>
+        <v>2489.327531709521</v>
       </c>
       <c r="P5" t="n">
         <v>2600.061856959047</v>
@@ -4592,25 +4592,25 @@
         <v>2635.045976980643</v>
       </c>
       <c r="S5" t="n">
-        <v>2478.830939477471</v>
+        <v>2635.045976980643</v>
       </c>
       <c r="T5" t="n">
-        <v>2264.031077745182</v>
+        <v>2635.045976980643</v>
       </c>
       <c r="U5" t="n">
-        <v>2010.339374490333</v>
+        <v>2405.315936268277</v>
       </c>
       <c r="V5" t="n">
-        <v>2010.339374490333</v>
+        <v>2074.253048924706</v>
       </c>
       <c r="W5" t="n">
-        <v>2010.339374490333</v>
+        <v>2074.253048924706</v>
       </c>
       <c r="X5" t="n">
-        <v>1656.31157281971</v>
+        <v>2074.253048924706</v>
       </c>
       <c r="Y5" t="n">
-        <v>1266.172240843898</v>
+        <v>2074.253048924706</v>
       </c>
     </row>
     <row r="6">
@@ -4699,28 +4699,28 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>70.57550729897547</v>
+        <v>280.5443918580929</v>
       </c>
       <c r="C7" t="n">
-        <v>70.57550729897547</v>
+        <v>280.5443918580929</v>
       </c>
       <c r="D7" t="n">
-        <v>70.57550729897547</v>
+        <v>280.5443918580929</v>
       </c>
       <c r="E7" t="n">
-        <v>70.57550729897547</v>
+        <v>132.6312982756997</v>
       </c>
       <c r="F7" t="n">
-        <v>70.57550729897547</v>
+        <v>52.70091953961285</v>
       </c>
       <c r="G7" t="n">
-        <v>70.57550729897547</v>
+        <v>52.70091953961285</v>
       </c>
       <c r="H7" t="n">
-        <v>70.57550729897547</v>
+        <v>52.70091953961285</v>
       </c>
       <c r="I7" t="n">
-        <v>70.57550729897547</v>
+        <v>52.70091953961285</v>
       </c>
       <c r="J7" t="n">
         <v>52.70091953961285</v>
@@ -4756,19 +4756,19 @@
         <v>1052.635600998958</v>
       </c>
       <c r="U7" t="n">
-        <v>808.7748073774835</v>
+        <v>1052.635600998958</v>
       </c>
       <c r="V7" t="n">
-        <v>808.7748073774835</v>
+        <v>797.9511127930708</v>
       </c>
       <c r="W7" t="n">
-        <v>519.3576373405228</v>
+        <v>508.5339427561102</v>
       </c>
       <c r="X7" t="n">
-        <v>291.3680864425056</v>
+        <v>280.5443918580929</v>
       </c>
       <c r="Y7" t="n">
-        <v>70.57550729897547</v>
+        <v>280.5443918580929</v>
       </c>
     </row>
     <row r="8">
@@ -4778,25 +4778,25 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>972.8094823977774</v>
+        <v>1371.028880093966</v>
       </c>
       <c r="C8" t="n">
-        <v>603.8469654573657</v>
+        <v>1002.066363153555</v>
       </c>
       <c r="D8" t="n">
-        <v>603.8469654573657</v>
+        <v>643.8006645468042</v>
       </c>
       <c r="E8" t="n">
-        <v>218.0587128591215</v>
+        <v>643.8006645468042</v>
       </c>
       <c r="F8" t="n">
-        <v>211.113212109918</v>
+        <v>636.8551637976008</v>
       </c>
       <c r="G8" t="n">
-        <v>198.0658343867495</v>
+        <v>219.7673820340282</v>
       </c>
       <c r="H8" t="n">
-        <v>52.70091953961285</v>
+        <v>172.393890139502</v>
       </c>
       <c r="I8" t="n">
         <v>52.70091953961285</v>
@@ -4829,25 +4829,25 @@
         <v>2635.045976980643</v>
       </c>
       <c r="S8" t="n">
-        <v>2635.045976980643</v>
+        <v>2478.830939477471</v>
       </c>
       <c r="T8" t="n">
-        <v>2420.246115248354</v>
+        <v>2478.830939477471</v>
       </c>
       <c r="U8" t="n">
-        <v>2420.246115248354</v>
+        <v>2478.830939477471</v>
       </c>
       <c r="V8" t="n">
-        <v>2089.183227904783</v>
+        <v>2147.7680521339</v>
       </c>
       <c r="W8" t="n">
-        <v>1736.414572634669</v>
+        <v>2147.7680521339</v>
       </c>
       <c r="X8" t="n">
-        <v>1362.948814373589</v>
+        <v>2147.7680521339</v>
       </c>
       <c r="Y8" t="n">
-        <v>972.8094823977774</v>
+        <v>1757.628720158088</v>
       </c>
     </row>
     <row r="9">
@@ -4887,16 +4887,16 @@
         <v>500.7885757023184</v>
       </c>
       <c r="L9" t="n">
-        <v>638.0181737180123</v>
+        <v>1005.150115568437</v>
       </c>
       <c r="M9" t="n">
-        <v>1278.563523185117</v>
+        <v>1232.27200203395</v>
       </c>
       <c r="N9" t="n">
-        <v>1746.206884640153</v>
+        <v>1430.928743686615</v>
       </c>
       <c r="O9" t="n">
-        <v>2295.642893392876</v>
+        <v>1980.364752439338</v>
       </c>
       <c r="P9" t="n">
         <v>2404.332520920175</v>
@@ -4936,28 +4936,28 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>52.70091953961285</v>
+        <v>446.6805723689433</v>
       </c>
       <c r="C10" t="n">
-        <v>52.70091953961285</v>
+        <v>446.6805723689433</v>
       </c>
       <c r="D10" t="n">
-        <v>52.70091953961285</v>
+        <v>446.6805723689433</v>
       </c>
       <c r="E10" t="n">
-        <v>52.70091953961285</v>
+        <v>446.6805723689433</v>
       </c>
       <c r="F10" t="n">
-        <v>52.70091953961285</v>
+        <v>393.436995403827</v>
       </c>
       <c r="G10" t="n">
-        <v>52.70091953961285</v>
+        <v>224.8301503992104</v>
       </c>
       <c r="H10" t="n">
-        <v>52.70091953961285</v>
+        <v>70.57550729897547</v>
       </c>
       <c r="I10" t="n">
-        <v>52.70091953961285</v>
+        <v>70.57550729897547</v>
       </c>
       <c r="J10" t="n">
         <v>52.70091953961285</v>
@@ -4987,25 +4987,25 @@
         <v>922.1576397183603</v>
       </c>
       <c r="S10" t="n">
-        <v>717.0234234737568</v>
+        <v>922.1576397183603</v>
       </c>
       <c r="T10" t="n">
-        <v>717.0234234737568</v>
+        <v>922.1576397183603</v>
       </c>
       <c r="U10" t="n">
-        <v>717.0234234737568</v>
+        <v>922.1576397183603</v>
       </c>
       <c r="V10" t="n">
-        <v>462.3389352678699</v>
+        <v>667.4731515124735</v>
       </c>
       <c r="W10" t="n">
-        <v>462.3389352678699</v>
+        <v>667.4731515124735</v>
       </c>
       <c r="X10" t="n">
-        <v>234.3493843698525</v>
+        <v>667.4731515124735</v>
       </c>
       <c r="Y10" t="n">
-        <v>234.3493843698525</v>
+        <v>446.6805723689433</v>
       </c>
     </row>
     <row r="11">
@@ -5033,16 +5033,16 @@
         <v>379.8308874362686</v>
       </c>
       <c r="H11" t="n">
-        <v>93.81666304797186</v>
+        <v>93.81666304797187</v>
       </c>
       <c r="I11" t="n">
-        <v>95.34095638192593</v>
+        <v>95.34095638192595</v>
       </c>
       <c r="J11" t="n">
-        <v>378.1925803111712</v>
+        <v>378.1925803111715</v>
       </c>
       <c r="K11" t="n">
-        <v>852.8523611075805</v>
+        <v>852.8523611075807</v>
       </c>
       <c r="L11" t="n">
         <v>1478.611553332387</v>
@@ -5060,19 +5060,19 @@
         <v>4194.413870694707</v>
       </c>
       <c r="Q11" t="n">
-        <v>4562.265728852254</v>
+        <v>4562.265728852255</v>
       </c>
       <c r="R11" t="n">
         <v>4690.833152398593</v>
       </c>
       <c r="S11" t="n">
-        <v>4606.285157492577</v>
+        <v>4606.285157492578</v>
       </c>
       <c r="T11" t="n">
-        <v>4405.252601474783</v>
+        <v>4405.252601474784</v>
       </c>
       <c r="U11" t="n">
-        <v>4151.812499466572</v>
+        <v>4151.812499466573</v>
       </c>
       <c r="V11" t="n">
         <v>3820.749612123003</v>
@@ -5112,31 +5112,31 @@
         <v>178.4809954028057</v>
       </c>
       <c r="H12" t="n">
-        <v>93.81666304797186</v>
+        <v>93.81666304797187</v>
       </c>
       <c r="I12" t="n">
-        <v>93.81666304797186</v>
+        <v>95.58405025273903</v>
       </c>
       <c r="J12" t="n">
-        <v>243.4633055756266</v>
+        <v>245.2306927803937</v>
       </c>
       <c r="K12" t="n">
-        <v>577.3880777468471</v>
+        <v>579.1554649516142</v>
       </c>
       <c r="L12" t="n">
-        <v>1072.713683962606</v>
+        <v>1074.481071167373</v>
       </c>
       <c r="M12" t="n">
-        <v>1670.092171589158</v>
+        <v>1671.859558793925</v>
       </c>
       <c r="N12" t="n">
-        <v>1670.092171589158</v>
+        <v>2299.457522348532</v>
       </c>
       <c r="O12" t="n">
-        <v>1896.176478190825</v>
+        <v>2553.061288060775</v>
       </c>
       <c r="P12" t="n">
-        <v>2319.799627685893</v>
+        <v>2553.061288060775</v>
       </c>
       <c r="Q12" t="n">
         <v>2553.061288060775</v>
@@ -5173,28 +5173,28 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>513.8536007400712</v>
+        <v>636.6680198981028</v>
       </c>
       <c r="C13" t="n">
-        <v>344.9174178121643</v>
+        <v>467.7318369701959</v>
       </c>
       <c r="D13" t="n">
-        <v>344.9174178121643</v>
+        <v>317.6151975578602</v>
       </c>
       <c r="E13" t="n">
-        <v>344.9174178121643</v>
+        <v>317.6151975578602</v>
       </c>
       <c r="F13" t="n">
-        <v>344.9174178121643</v>
+        <v>317.6151975578602</v>
       </c>
       <c r="G13" t="n">
-        <v>317.6151975578601</v>
+        <v>317.6151975578602</v>
       </c>
       <c r="H13" t="n">
-        <v>175.9033664000582</v>
+        <v>175.9033664000583</v>
       </c>
       <c r="I13" t="n">
-        <v>93.81666304797186</v>
+        <v>93.81666304797187</v>
       </c>
       <c r="J13" t="n">
         <v>174.0526814782957</v>
@@ -5236,13 +5236,13 @@
         <v>1433.701365648819</v>
       </c>
       <c r="W13" t="n">
-        <v>1144.284195611858</v>
+        <v>1267.09861476989</v>
       </c>
       <c r="X13" t="n">
-        <v>916.2946447138411</v>
+        <v>1039.109063871873</v>
       </c>
       <c r="Y13" t="n">
-        <v>695.5020655703109</v>
+        <v>818.3164847283425</v>
       </c>
     </row>
     <row r="14">
@@ -5252,37 +5252,37 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>2317.776026551874</v>
+        <v>2317.776026551875</v>
       </c>
       <c r="C14" t="n">
-        <v>1948.813509611462</v>
+        <v>1948.813509611463</v>
       </c>
       <c r="D14" t="n">
-        <v>1590.547811004712</v>
+        <v>1590.547811004713</v>
       </c>
       <c r="E14" t="n">
-        <v>1204.759558406468</v>
+        <v>1204.759558406469</v>
       </c>
       <c r="F14" t="n">
-        <v>793.7736536168605</v>
+        <v>793.7736536168611</v>
       </c>
       <c r="G14" t="n">
         <v>379.8308874362686</v>
       </c>
       <c r="H14" t="n">
-        <v>93.81666304797186</v>
+        <v>93.81666304797187</v>
       </c>
       <c r="I14" t="n">
-        <v>95.34095638192593</v>
+        <v>95.34095638192616</v>
       </c>
       <c r="J14" t="n">
-        <v>378.1925803111711</v>
+        <v>378.1925803111717</v>
       </c>
       <c r="K14" t="n">
-        <v>852.8523611075804</v>
+        <v>852.8523611075809</v>
       </c>
       <c r="L14" t="n">
-        <v>1478.611553332386</v>
+        <v>1478.611553332387</v>
       </c>
       <c r="M14" t="n">
         <v>2206.558663014778</v>
@@ -5294,34 +5294,34 @@
         <v>3640.422291068009</v>
       </c>
       <c r="P14" t="n">
-        <v>4194.413870694706</v>
+        <v>4194.413870694707</v>
       </c>
       <c r="Q14" t="n">
-        <v>4562.265728852254</v>
+        <v>4562.265728852255</v>
       </c>
       <c r="R14" t="n">
         <v>4690.833152398593</v>
       </c>
       <c r="S14" t="n">
-        <v>4606.285157492577</v>
+        <v>4606.285157492578</v>
       </c>
       <c r="T14" t="n">
-        <v>4405.252601474783</v>
+        <v>4405.252601474784</v>
       </c>
       <c r="U14" t="n">
-        <v>4151.812499466572</v>
+        <v>4151.812499466573</v>
       </c>
       <c r="V14" t="n">
-        <v>3820.749612123001</v>
+        <v>3820.749612123002</v>
       </c>
       <c r="W14" t="n">
-        <v>3467.980956852887</v>
+        <v>3467.980956852888</v>
       </c>
       <c r="X14" t="n">
-        <v>3094.515198591807</v>
+        <v>3094.515198591808</v>
       </c>
       <c r="Y14" t="n">
-        <v>2704.375866615996</v>
+        <v>2704.375866615997</v>
       </c>
     </row>
     <row r="15">
@@ -5349,31 +5349,31 @@
         <v>178.4809954028057</v>
       </c>
       <c r="H15" t="n">
-        <v>93.81666304797186</v>
+        <v>93.81666304797187</v>
       </c>
       <c r="I15" t="n">
-        <v>93.81666304797186</v>
+        <v>95.58405025273903</v>
       </c>
       <c r="J15" t="n">
-        <v>243.4633055756266</v>
+        <v>245.2306927803937</v>
       </c>
       <c r="K15" t="n">
-        <v>577.3880777468471</v>
+        <v>579.1554649516142</v>
       </c>
       <c r="L15" t="n">
-        <v>1072.713683962606</v>
+        <v>1074.481071167373</v>
       </c>
       <c r="M15" t="n">
-        <v>1670.092171589158</v>
+        <v>1671.859558793925</v>
       </c>
       <c r="N15" t="n">
-        <v>1896.176478190825</v>
+        <v>2299.457522348532</v>
       </c>
       <c r="O15" t="n">
-        <v>1896.176478190825</v>
+        <v>2553.061288060775</v>
       </c>
       <c r="P15" t="n">
-        <v>2319.799627685893</v>
+        <v>2553.061288060775</v>
       </c>
       <c r="Q15" t="n">
         <v>2553.061288060775</v>
@@ -5410,28 +5410,28 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>951.7772127656159</v>
+        <v>653.7474797708871</v>
       </c>
       <c r="C16" t="n">
-        <v>782.841029837709</v>
+        <v>484.8112968429803</v>
       </c>
       <c r="D16" t="n">
-        <v>632.7243904253733</v>
+        <v>484.8112968429803</v>
       </c>
       <c r="E16" t="n">
-        <v>484.8112968429802</v>
+        <v>484.8112968429803</v>
       </c>
       <c r="F16" t="n">
-        <v>484.8112968429802</v>
+        <v>484.8112968429803</v>
       </c>
       <c r="G16" t="n">
-        <v>317.6151975578601</v>
+        <v>317.6151975578602</v>
       </c>
       <c r="H16" t="n">
-        <v>175.9033664000582</v>
+        <v>175.9033664000583</v>
       </c>
       <c r="I16" t="n">
-        <v>93.81666304797186</v>
+        <v>93.81666304797187</v>
       </c>
       <c r="J16" t="n">
         <v>174.0526814782957</v>
@@ -5461,25 +5461,25 @@
         <v>2379.917379832663</v>
       </c>
       <c r="S16" t="n">
-        <v>2379.917379832663</v>
+        <v>2197.062545487567</v>
       </c>
       <c r="T16" t="n">
-        <v>2160.315914855604</v>
+        <v>2117.354959541324</v>
       </c>
       <c r="U16" t="n">
-        <v>1871.240688199802</v>
+        <v>1828.279732885522</v>
       </c>
       <c r="V16" t="n">
-        <v>1616.556199993915</v>
+        <v>1573.595244679635</v>
       </c>
       <c r="W16" t="n">
-        <v>1327.139029956954</v>
+        <v>1284.178074642674</v>
       </c>
       <c r="X16" t="n">
-        <v>1133.425677595856</v>
+        <v>1056.188523744657</v>
       </c>
       <c r="Y16" t="n">
-        <v>1133.425677595856</v>
+        <v>835.3959446011269</v>
       </c>
     </row>
     <row r="17">
@@ -5489,34 +5489,34 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>2317.776026551874</v>
+        <v>2317.776026551875</v>
       </c>
       <c r="C17" t="n">
-        <v>1948.813509611462</v>
+        <v>1948.813509611463</v>
       </c>
       <c r="D17" t="n">
-        <v>1590.547811004712</v>
+        <v>1590.547811004713</v>
       </c>
       <c r="E17" t="n">
-        <v>1204.759558406467</v>
+        <v>1204.759558406469</v>
       </c>
       <c r="F17" t="n">
-        <v>793.7736536168597</v>
+        <v>793.7736536168611</v>
       </c>
       <c r="G17" t="n">
         <v>379.8308874362686</v>
       </c>
       <c r="H17" t="n">
-        <v>93.81666304797186</v>
+        <v>93.81666304797187</v>
       </c>
       <c r="I17" t="n">
-        <v>95.34095638192593</v>
+        <v>95.34095638192616</v>
       </c>
       <c r="J17" t="n">
-        <v>378.1925803111715</v>
+        <v>378.1925803111717</v>
       </c>
       <c r="K17" t="n">
-        <v>852.8523611075807</v>
+        <v>852.8523611075809</v>
       </c>
       <c r="L17" t="n">
         <v>1478.611553332387</v>
@@ -5528,7 +5528,7 @@
         <v>2950.898526355937</v>
       </c>
       <c r="O17" t="n">
-        <v>3640.422291068009</v>
+        <v>3640.42229106801</v>
       </c>
       <c r="P17" t="n">
         <v>4194.413870694707</v>
@@ -5540,25 +5540,25 @@
         <v>4690.833152398593</v>
       </c>
       <c r="S17" t="n">
-        <v>4606.285157492577</v>
+        <v>4606.285157492578</v>
       </c>
       <c r="T17" t="n">
-        <v>4405.252601474783</v>
+        <v>4405.252601474784</v>
       </c>
       <c r="U17" t="n">
-        <v>4151.812499466572</v>
+        <v>4151.812499466573</v>
       </c>
       <c r="V17" t="n">
-        <v>3820.749612123001</v>
+        <v>3820.749612123002</v>
       </c>
       <c r="W17" t="n">
-        <v>3467.980956852887</v>
+        <v>3467.980956852888</v>
       </c>
       <c r="X17" t="n">
-        <v>3094.515198591807</v>
+        <v>3094.515198591808</v>
       </c>
       <c r="Y17" t="n">
-        <v>2704.375866615996</v>
+        <v>2704.375866615997</v>
       </c>
     </row>
     <row r="18">
@@ -5586,22 +5586,22 @@
         <v>178.4809954028057</v>
       </c>
       <c r="H18" t="n">
-        <v>93.81666304797186</v>
+        <v>93.81666304797187</v>
       </c>
       <c r="I18" t="n">
-        <v>93.81666304797186</v>
+        <v>95.58405025273903</v>
       </c>
       <c r="J18" t="n">
-        <v>243.4633055756266</v>
+        <v>245.2306927803937</v>
       </c>
       <c r="K18" t="n">
-        <v>577.3880777468471</v>
+        <v>579.1554649516142</v>
       </c>
       <c r="L18" t="n">
-        <v>1072.713683962606</v>
+        <v>1074.481071167373</v>
       </c>
       <c r="M18" t="n">
-        <v>1670.092171589158</v>
+        <v>1671.859558793925</v>
       </c>
       <c r="N18" t="n">
         <v>1859.536823237711</v>
@@ -5647,28 +5647,28 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>580.8993044876688</v>
+        <v>571.6607764188008</v>
       </c>
       <c r="C19" t="n">
-        <v>411.9631215597619</v>
+        <v>402.7245934908939</v>
       </c>
       <c r="D19" t="n">
-        <v>411.9631215597619</v>
+        <v>402.7245934908939</v>
       </c>
       <c r="E19" t="n">
-        <v>411.9631215597619</v>
+        <v>402.7245934908939</v>
       </c>
       <c r="F19" t="n">
-        <v>265.0731740618515</v>
+        <v>402.7245934908939</v>
       </c>
       <c r="G19" t="n">
-        <v>97.87707477673149</v>
+        <v>235.5284942057738</v>
       </c>
       <c r="H19" t="n">
-        <v>97.87707477673149</v>
+        <v>93.81666304797187</v>
       </c>
       <c r="I19" t="n">
-        <v>93.81666304797186</v>
+        <v>93.81666304797187</v>
       </c>
       <c r="J19" t="n">
         <v>174.0526814782957</v>
@@ -5695,28 +5695,28 @@
         <v>2446.96308358026</v>
       </c>
       <c r="R19" t="n">
-        <v>2446.96308358026</v>
+        <v>2379.917379832663</v>
       </c>
       <c r="S19" t="n">
-        <v>2264.108249235165</v>
+        <v>2197.062545487567</v>
       </c>
       <c r="T19" t="n">
-        <v>2044.506784258106</v>
+        <v>1977.461080510508</v>
       </c>
       <c r="U19" t="n">
-        <v>1755.431557602304</v>
+        <v>1688.385853854706</v>
       </c>
       <c r="V19" t="n">
-        <v>1500.747069396417</v>
+        <v>1433.701365648819</v>
       </c>
       <c r="W19" t="n">
-        <v>1211.329899359456</v>
+        <v>1202.091371290588</v>
       </c>
       <c r="X19" t="n">
-        <v>983.3403484614387</v>
+        <v>974.1018203925706</v>
       </c>
       <c r="Y19" t="n">
-        <v>762.5477693179085</v>
+        <v>753.3092412490405</v>
       </c>
     </row>
     <row r="20">
@@ -5744,10 +5744,10 @@
         <v>379.8308874362686</v>
       </c>
       <c r="H20" t="n">
-        <v>93.81666304797186</v>
+        <v>93.81666304797187</v>
       </c>
       <c r="I20" t="n">
-        <v>95.34095638192599</v>
+        <v>95.34095638192595</v>
       </c>
       <c r="J20" t="n">
         <v>378.1925803111715</v>
@@ -5765,13 +5765,13 @@
         <v>2950.898526355937</v>
       </c>
       <c r="O20" t="n">
-        <v>3640.42229106801</v>
+        <v>3640.422291068009</v>
       </c>
       <c r="P20" t="n">
         <v>4194.413870694707</v>
       </c>
       <c r="Q20" t="n">
-        <v>4562.265728852254</v>
+        <v>4562.265728852255</v>
       </c>
       <c r="R20" t="n">
         <v>4690.833152398593</v>
@@ -5823,10 +5823,10 @@
         <v>178.4809954028057</v>
       </c>
       <c r="H21" t="n">
-        <v>93.81666304797186</v>
+        <v>93.81666304797187</v>
       </c>
       <c r="I21" t="n">
-        <v>95.58405025273902</v>
+        <v>95.58405025273903</v>
       </c>
       <c r="J21" t="n">
         <v>245.2306927803937</v>
@@ -5838,19 +5838,19 @@
         <v>1074.481071167373</v>
       </c>
       <c r="M21" t="n">
-        <v>1671.859558793925</v>
+        <v>1501.8401750111</v>
       </c>
       <c r="N21" t="n">
-        <v>2299.457522348532</v>
+        <v>2129.438138565707</v>
       </c>
       <c r="O21" t="n">
-        <v>2516.421633107662</v>
+        <v>2129.438138565707</v>
       </c>
       <c r="P21" t="n">
-        <v>2516.421633107662</v>
+        <v>2553.061288060775</v>
       </c>
       <c r="Q21" t="n">
-        <v>2516.421633107662</v>
+        <v>2553.061288060775</v>
       </c>
       <c r="R21" t="n">
         <v>2553.061288060775</v>
@@ -5902,10 +5902,10 @@
         <v>235.5284942057738</v>
       </c>
       <c r="H22" t="n">
-        <v>93.81666304797186</v>
+        <v>93.81666304797187</v>
       </c>
       <c r="I22" t="n">
-        <v>93.81666304797186</v>
+        <v>93.81666304797187</v>
       </c>
       <c r="J22" t="n">
         <v>174.0526814782957</v>
@@ -5969,22 +5969,22 @@
         <v>1948.813509611463</v>
       </c>
       <c r="D23" t="n">
-        <v>1590.547811004713</v>
+        <v>1590.547811004712</v>
       </c>
       <c r="E23" t="n">
-        <v>1204.759558406469</v>
+        <v>1204.759558406468</v>
       </c>
       <c r="F23" t="n">
-        <v>793.7736536168611</v>
+        <v>793.7736536168607</v>
       </c>
       <c r="G23" t="n">
-        <v>379.8308874362686</v>
+        <v>379.8308874362681</v>
       </c>
       <c r="H23" t="n">
-        <v>93.81666304797186</v>
+        <v>93.81666304797187</v>
       </c>
       <c r="I23" t="n">
-        <v>95.34095638192593</v>
+        <v>95.34095638192595</v>
       </c>
       <c r="J23" t="n">
         <v>378.1925803111715</v>
@@ -5996,40 +5996,40 @@
         <v>1478.611553332387</v>
       </c>
       <c r="M23" t="n">
-        <v>2206.558663014778</v>
+        <v>2206.558663014779</v>
       </c>
       <c r="N23" t="n">
-        <v>2950.898526355936</v>
+        <v>2950.898526355937</v>
       </c>
       <c r="O23" t="n">
         <v>3640.422291068009</v>
       </c>
       <c r="P23" t="n">
-        <v>4194.413870694706</v>
+        <v>4194.413870694707</v>
       </c>
       <c r="Q23" t="n">
-        <v>4562.265728852254</v>
+        <v>4562.265728852255</v>
       </c>
       <c r="R23" t="n">
         <v>4690.833152398593</v>
       </c>
       <c r="S23" t="n">
-        <v>4606.285157492577</v>
+        <v>4606.285157492578</v>
       </c>
       <c r="T23" t="n">
-        <v>4405.252601474783</v>
+        <v>4405.252601474784</v>
       </c>
       <c r="U23" t="n">
         <v>4151.812499466573</v>
       </c>
       <c r="V23" t="n">
-        <v>3820.749612123003</v>
+        <v>3820.749612123002</v>
       </c>
       <c r="W23" t="n">
-        <v>3467.980956852889</v>
+        <v>3467.980956852888</v>
       </c>
       <c r="X23" t="n">
-        <v>3094.515198591809</v>
+        <v>3094.515198591808</v>
       </c>
       <c r="Y23" t="n">
         <v>2704.375866615997</v>
@@ -6060,10 +6060,10 @@
         <v>178.4809954028057</v>
       </c>
       <c r="H24" t="n">
-        <v>93.81666304797186</v>
+        <v>93.81666304797187</v>
       </c>
       <c r="I24" t="n">
-        <v>95.58405025273902</v>
+        <v>95.58405025273903</v>
       </c>
       <c r="J24" t="n">
         <v>245.2306927803937</v>
@@ -6078,13 +6078,13 @@
         <v>1671.859558793925</v>
       </c>
       <c r="N24" t="n">
-        <v>1671.859558793925</v>
+        <v>2299.457522348532</v>
       </c>
       <c r="O24" t="n">
-        <v>1896.176478190825</v>
+        <v>2553.061288060775</v>
       </c>
       <c r="P24" t="n">
-        <v>2319.799627685893</v>
+        <v>2553.061288060775</v>
       </c>
       <c r="Q24" t="n">
         <v>2553.061288060775</v>
@@ -6130,19 +6130,19 @@
         <v>344.9174178121643</v>
       </c>
       <c r="E25" t="n">
-        <v>197.0043242297712</v>
+        <v>344.9174178121643</v>
       </c>
       <c r="F25" t="n">
-        <v>197.0043242297712</v>
+        <v>344.9174178121643</v>
       </c>
       <c r="G25" t="n">
-        <v>93.81666304797186</v>
+        <v>235.5284942057738</v>
       </c>
       <c r="H25" t="n">
-        <v>93.81666304797186</v>
+        <v>93.81666304797187</v>
       </c>
       <c r="I25" t="n">
-        <v>93.81666304797186</v>
+        <v>93.81666304797187</v>
       </c>
       <c r="J25" t="n">
         <v>174.0526814782957</v>
@@ -6200,16 +6200,16 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>2317.776026551874</v>
+        <v>2317.776026551875</v>
       </c>
       <c r="C26" t="n">
-        <v>1948.813509611462</v>
+        <v>1948.813509611463</v>
       </c>
       <c r="D26" t="n">
-        <v>1590.547811004712</v>
+        <v>1590.547811004713</v>
       </c>
       <c r="E26" t="n">
-        <v>1204.759558406467</v>
+        <v>1204.759558406469</v>
       </c>
       <c r="F26" t="n">
         <v>793.7736536168611</v>
@@ -6306,25 +6306,25 @@
         <v>245.2306927803937</v>
       </c>
       <c r="K27" t="n">
-        <v>245.2306927803937</v>
+        <v>579.1554649516142</v>
       </c>
       <c r="L27" t="n">
-        <v>740.5562989961525</v>
+        <v>1074.481071167373</v>
       </c>
       <c r="M27" t="n">
-        <v>1337.934786622704</v>
+        <v>1671.859558793925</v>
       </c>
       <c r="N27" t="n">
-        <v>1965.532750177311</v>
+        <v>2299.457522348532</v>
       </c>
       <c r="O27" t="n">
-        <v>2516.421633107662</v>
+        <v>2553.061288060775</v>
       </c>
       <c r="P27" t="n">
-        <v>2516.421633107662</v>
+        <v>2553.061288060775</v>
       </c>
       <c r="Q27" t="n">
-        <v>2516.421633107662</v>
+        <v>2553.061288060775</v>
       </c>
       <c r="R27" t="n">
         <v>2553.061288060775</v>
@@ -6367,7 +6367,7 @@
         <v>656.964603115003</v>
       </c>
       <c r="E28" t="n">
-        <v>533.5814564942661</v>
+        <v>533.5814564942654</v>
       </c>
       <c r="F28" t="n">
         <v>411.2214559580113</v>
@@ -6546,13 +6546,13 @@
         <v>579.1554649516142</v>
       </c>
       <c r="L30" t="n">
-        <v>776.1751066403293</v>
+        <v>1074.481071167373</v>
       </c>
       <c r="M30" t="n">
-        <v>1373.553594266881</v>
+        <v>1671.859558793925</v>
       </c>
       <c r="N30" t="n">
-        <v>2001.151557821488</v>
+        <v>2299.457522348532</v>
       </c>
       <c r="O30" t="n">
         <v>2553.061288060775</v>
@@ -6601,10 +6601,10 @@
         <v>782.5512955656824</v>
       </c>
       <c r="D31" t="n">
-        <v>656.964603115003</v>
+        <v>656.9646031150022</v>
       </c>
       <c r="E31" t="n">
-        <v>533.5814564942661</v>
+        <v>533.5814564942654</v>
       </c>
       <c r="F31" t="n">
         <v>411.2214559580113</v>
@@ -6674,43 +6674,43 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>2317.776026551874</v>
+        <v>2317.776026551875</v>
       </c>
       <c r="C32" t="n">
-        <v>1948.813509611462</v>
+        <v>1948.813509611463</v>
       </c>
       <c r="D32" t="n">
-        <v>1590.547811004712</v>
+        <v>1590.547811004713</v>
       </c>
       <c r="E32" t="n">
-        <v>1204.759558406467</v>
+        <v>1204.759558406469</v>
       </c>
       <c r="F32" t="n">
-        <v>793.7736536168597</v>
+        <v>793.7736536168611</v>
       </c>
       <c r="G32" t="n">
         <v>379.8308874362686</v>
       </c>
       <c r="H32" t="n">
-        <v>93.81666304797186</v>
+        <v>93.81666304797187</v>
       </c>
       <c r="I32" t="n">
-        <v>95.34095638192599</v>
+        <v>95.34095638192616</v>
       </c>
       <c r="J32" t="n">
-        <v>378.1925803111715</v>
+        <v>378.1925803111717</v>
       </c>
       <c r="K32" t="n">
-        <v>852.8523611075802</v>
+        <v>852.8523611075809</v>
       </c>
       <c r="L32" t="n">
         <v>1478.611553332387</v>
       </c>
       <c r="M32" t="n">
-        <v>2206.558663014778</v>
+        <v>2206.558663014779</v>
       </c>
       <c r="N32" t="n">
-        <v>2950.898526355936</v>
+        <v>2950.898526355937</v>
       </c>
       <c r="O32" t="n">
         <v>3640.42229106801</v>
@@ -6719,31 +6719,31 @@
         <v>4194.413870694707</v>
       </c>
       <c r="Q32" t="n">
-        <v>4562.265728852254</v>
+        <v>4562.265728852255</v>
       </c>
       <c r="R32" t="n">
         <v>4690.833152398593</v>
       </c>
       <c r="S32" t="n">
-        <v>4606.285157492577</v>
+        <v>4606.285157492578</v>
       </c>
       <c r="T32" t="n">
-        <v>4405.252601474783</v>
+        <v>4405.252601474784</v>
       </c>
       <c r="U32" t="n">
-        <v>4151.812499466572</v>
+        <v>4151.812499466573</v>
       </c>
       <c r="V32" t="n">
-        <v>3820.749612123001</v>
+        <v>3820.749612123003</v>
       </c>
       <c r="W32" t="n">
-        <v>3467.980956852887</v>
+        <v>3467.980956852889</v>
       </c>
       <c r="X32" t="n">
-        <v>3094.515198591807</v>
+        <v>3094.515198591809</v>
       </c>
       <c r="Y32" t="n">
-        <v>2704.375866615996</v>
+        <v>2704.375866615997</v>
       </c>
     </row>
     <row r="33">
@@ -6771,10 +6771,10 @@
         <v>178.4809954028057</v>
       </c>
       <c r="H33" t="n">
-        <v>93.81666304797186</v>
+        <v>93.81666304797187</v>
       </c>
       <c r="I33" t="n">
-        <v>95.58405025273902</v>
+        <v>95.58405025273903</v>
       </c>
       <c r="J33" t="n">
         <v>245.2306927803937</v>
@@ -6847,22 +6847,22 @@
         <v>411.2214559580118</v>
       </c>
       <c r="G34" t="n">
-        <v>268.5553036345475</v>
+        <v>268.555303634547</v>
       </c>
       <c r="H34" t="n">
-        <v>151.3734194384019</v>
+        <v>151.373419438402</v>
       </c>
       <c r="I34" t="n">
-        <v>93.81666304797186</v>
+        <v>93.81666304797189</v>
       </c>
       <c r="J34" t="n">
-        <v>198.094482495415</v>
+        <v>198.0944824954151</v>
       </c>
       <c r="K34" t="n">
-        <v>483.8255460380729</v>
+        <v>483.825546038073</v>
       </c>
       <c r="L34" t="n">
-        <v>898.2659412311324</v>
+        <v>898.2659412311325</v>
       </c>
       <c r="M34" t="n">
         <v>1344.317444979286</v>
@@ -6917,7 +6917,7 @@
         <v>1948.813509611463</v>
       </c>
       <c r="D35" t="n">
-        <v>1590.547811004712</v>
+        <v>1590.547811004713</v>
       </c>
       <c r="E35" t="n">
         <v>1204.759558406469</v>
@@ -6929,25 +6929,25 @@
         <v>379.8308874362686</v>
       </c>
       <c r="H35" t="n">
-        <v>93.81666304797187</v>
+        <v>93.81666304797186</v>
       </c>
       <c r="I35" t="n">
-        <v>95.34095638192593</v>
+        <v>95.34095638192599</v>
       </c>
       <c r="J35" t="n">
-        <v>378.1925803111712</v>
+        <v>378.1925803111715</v>
       </c>
       <c r="K35" t="n">
-        <v>852.8523611075805</v>
+        <v>852.8523611075802</v>
       </c>
       <c r="L35" t="n">
         <v>1478.611553332387</v>
       </c>
       <c r="M35" t="n">
-        <v>2206.558663014779</v>
+        <v>2206.558663014778</v>
       </c>
       <c r="N35" t="n">
-        <v>2950.898526355937</v>
+        <v>2950.898526355936</v>
       </c>
       <c r="O35" t="n">
         <v>3640.42229106801</v>
@@ -6956,28 +6956,28 @@
         <v>4194.413870694707</v>
       </c>
       <c r="Q35" t="n">
-        <v>4562.265728852255</v>
+        <v>4562.265728852254</v>
       </c>
       <c r="R35" t="n">
         <v>4690.833152398593</v>
       </c>
       <c r="S35" t="n">
-        <v>4606.285157492578</v>
+        <v>4606.285157492577</v>
       </c>
       <c r="T35" t="n">
-        <v>4405.252601474784</v>
+        <v>4405.252601474783</v>
       </c>
       <c r="U35" t="n">
         <v>4151.812499466573</v>
       </c>
       <c r="V35" t="n">
-        <v>3820.749612123002</v>
+        <v>3820.749612123003</v>
       </c>
       <c r="W35" t="n">
-        <v>3467.980956852888</v>
+        <v>3467.980956852889</v>
       </c>
       <c r="X35" t="n">
-        <v>3094.515198591808</v>
+        <v>3094.515198591809</v>
       </c>
       <c r="Y35" t="n">
         <v>2704.375866615997</v>
@@ -7008,10 +7008,10 @@
         <v>178.4809954028057</v>
       </c>
       <c r="H36" t="n">
-        <v>93.81666304797187</v>
+        <v>93.81666304797186</v>
       </c>
       <c r="I36" t="n">
-        <v>95.58405025273903</v>
+        <v>95.58405025273902</v>
       </c>
       <c r="J36" t="n">
         <v>245.2306927803937</v>
@@ -7069,37 +7069,37 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>926.9575315319325</v>
+        <v>926.9575315319323</v>
       </c>
       <c r="C37" t="n">
-        <v>782.5512955656819</v>
+        <v>782.5512955656816</v>
       </c>
       <c r="D37" t="n">
-        <v>656.9646031150025</v>
+        <v>656.9646031150021</v>
       </c>
       <c r="E37" t="n">
-        <v>533.5814564942657</v>
+        <v>533.5814564942655</v>
       </c>
       <c r="F37" t="n">
-        <v>411.2214559580117</v>
+        <v>411.2214559580115</v>
       </c>
       <c r="G37" t="n">
-        <v>268.5553036345476</v>
+        <v>268.5553036345477</v>
       </c>
       <c r="H37" t="n">
         <v>151.373419438402</v>
       </c>
       <c r="I37" t="n">
-        <v>93.81666304797189</v>
+        <v>93.81666304797186</v>
       </c>
       <c r="J37" t="n">
         <v>198.094482495415</v>
       </c>
       <c r="K37" t="n">
-        <v>483.825546038073</v>
+        <v>483.8255460380728</v>
       </c>
       <c r="L37" t="n">
-        <v>898.2659412311324</v>
+        <v>898.2659412311323</v>
       </c>
       <c r="M37" t="n">
         <v>1344.317444979286</v>
@@ -7108,19 +7108,19 @@
         <v>1785.769117656414</v>
       </c>
       <c r="O37" t="n">
-        <v>2179.340199382519</v>
+        <v>2179.340199382518</v>
       </c>
       <c r="P37" t="n">
-        <v>2496.057455973197</v>
+        <v>2496.057455973196</v>
       </c>
       <c r="Q37" t="n">
         <v>2639.297491717215</v>
       </c>
       <c r="R37" t="n">
-        <v>2596.781734931274</v>
+        <v>2596.781734931273</v>
       </c>
       <c r="S37" t="n">
-        <v>2438.456847547835</v>
+        <v>2438.456847547834</v>
       </c>
       <c r="T37" t="n">
         <v>2243.385329532432</v>
@@ -7172,10 +7172,10 @@
         <v>95.34095638192593</v>
       </c>
       <c r="J38" t="n">
-        <v>378.1925803111712</v>
+        <v>378.192580311172</v>
       </c>
       <c r="K38" t="n">
-        <v>852.8523611075805</v>
+        <v>852.8523611075813</v>
       </c>
       <c r="L38" t="n">
         <v>1478.611553332387</v>
@@ -7306,37 +7306,37 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>926.9575315319328</v>
+        <v>926.9575315319322</v>
       </c>
       <c r="C40" t="n">
-        <v>782.551295565682</v>
+        <v>782.5512955656816</v>
       </c>
       <c r="D40" t="n">
-        <v>656.9646031150025</v>
+        <v>656.9646031150021</v>
       </c>
       <c r="E40" t="n">
-        <v>533.5814564942657</v>
+        <v>533.5814564942652</v>
       </c>
       <c r="F40" t="n">
-        <v>411.2214559580116</v>
+        <v>411.2214559580113</v>
       </c>
       <c r="G40" t="n">
-        <v>268.5553036345477</v>
+        <v>268.5553036345476</v>
       </c>
       <c r="H40" t="n">
         <v>151.373419438402</v>
       </c>
       <c r="I40" t="n">
-        <v>93.81666304797189</v>
+        <v>93.81666304797186</v>
       </c>
       <c r="J40" t="n">
-        <v>198.094482495415</v>
+        <v>198.0944824954149</v>
       </c>
       <c r="K40" t="n">
         <v>483.8255460380728</v>
       </c>
       <c r="L40" t="n">
-        <v>898.2659412311322</v>
+        <v>898.2659412311323</v>
       </c>
       <c r="M40" t="n">
         <v>1344.317444979286</v>
@@ -7354,25 +7354,25 @@
         <v>2639.297491717215</v>
       </c>
       <c r="R40" t="n">
-        <v>2596.781734931274</v>
+        <v>2596.781734931273</v>
       </c>
       <c r="S40" t="n">
         <v>2438.456847547834</v>
       </c>
       <c r="T40" t="n">
-        <v>2243.385329532432</v>
+        <v>2243.385329532431</v>
       </c>
       <c r="U40" t="n">
-        <v>1978.840049838286</v>
+        <v>1978.840049838285</v>
       </c>
       <c r="V40" t="n">
-        <v>1748.685508594056</v>
+        <v>1748.685508594055</v>
       </c>
       <c r="W40" t="n">
-        <v>1483.798285518751</v>
+        <v>1483.79828551875</v>
       </c>
       <c r="X40" t="n">
-        <v>1280.33868158239</v>
+        <v>1280.338681582389</v>
       </c>
       <c r="Y40" t="n">
         <v>1084.076049400516</v>
@@ -7385,19 +7385,19 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>2317.776026551875</v>
+        <v>2317.776026551874</v>
       </c>
       <c r="C41" t="n">
-        <v>1948.813509611463</v>
+        <v>1948.813509611462</v>
       </c>
       <c r="D41" t="n">
-        <v>1590.547811004713</v>
+        <v>1590.547811004712</v>
       </c>
       <c r="E41" t="n">
-        <v>1204.759558406469</v>
+        <v>1204.759558406468</v>
       </c>
       <c r="F41" t="n">
-        <v>793.7736536168611</v>
+        <v>793.7736536168609</v>
       </c>
       <c r="G41" t="n">
         <v>379.8308874362686</v>
@@ -7406,13 +7406,13 @@
         <v>93.81666304797187</v>
       </c>
       <c r="I41" t="n">
-        <v>95.34095638192593</v>
+        <v>95.34095638192595</v>
       </c>
       <c r="J41" t="n">
-        <v>378.192580311172</v>
+        <v>378.1925803111715</v>
       </c>
       <c r="K41" t="n">
-        <v>852.8523611075813</v>
+        <v>852.8523611075807</v>
       </c>
       <c r="L41" t="n">
         <v>1478.611553332387</v>
@@ -7424,7 +7424,7 @@
         <v>2950.898526355937</v>
       </c>
       <c r="O41" t="n">
-        <v>3640.42229106801</v>
+        <v>3640.422291068009</v>
       </c>
       <c r="P41" t="n">
         <v>4194.413870694707</v>
@@ -7442,19 +7442,19 @@
         <v>4405.252601474784</v>
       </c>
       <c r="U41" t="n">
-        <v>4151.812499466573</v>
+        <v>4151.812499466572</v>
       </c>
       <c r="V41" t="n">
-        <v>3820.749612123002</v>
+        <v>3820.749612123001</v>
       </c>
       <c r="W41" t="n">
-        <v>3467.980956852888</v>
+        <v>3467.980956852887</v>
       </c>
       <c r="X41" t="n">
-        <v>3094.515198591808</v>
+        <v>3094.515198591807</v>
       </c>
       <c r="Y41" t="n">
-        <v>2704.375866615997</v>
+        <v>2704.375866615996</v>
       </c>
     </row>
     <row r="42">
@@ -7485,31 +7485,31 @@
         <v>93.81666304797187</v>
       </c>
       <c r="I42" t="n">
-        <v>93.81666304797187</v>
+        <v>95.58405025273903</v>
       </c>
       <c r="J42" t="n">
-        <v>93.81666304797187</v>
+        <v>245.2306927803937</v>
       </c>
       <c r="K42" t="n">
-        <v>93.81666304797187</v>
+        <v>579.1554649516142</v>
       </c>
       <c r="L42" t="n">
-        <v>93.81666304797187</v>
+        <v>1074.481071167373</v>
       </c>
       <c r="M42" t="n">
-        <v>680.0291294438176</v>
+        <v>1671.859558793925</v>
       </c>
       <c r="N42" t="n">
-        <v>1307.627092998424</v>
+        <v>2299.457522348532</v>
       </c>
       <c r="O42" t="n">
-        <v>1859.536823237711</v>
+        <v>2553.061288060775</v>
       </c>
       <c r="P42" t="n">
-        <v>2283.159972732779</v>
+        <v>2553.061288060775</v>
       </c>
       <c r="Q42" t="n">
-        <v>2516.421633107662</v>
+        <v>2553.061288060775</v>
       </c>
       <c r="R42" t="n">
         <v>2553.061288060775</v>
@@ -7543,28 +7543,28 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>926.9575315319324</v>
+        <v>926.9575315319317</v>
       </c>
       <c r="C43" t="n">
-        <v>782.5512955656818</v>
+        <v>782.5512955656811</v>
       </c>
       <c r="D43" t="n">
-        <v>656.9646031150023</v>
+        <v>656.9646031150016</v>
       </c>
       <c r="E43" t="n">
-        <v>533.5814564942655</v>
+        <v>533.5814564942648</v>
       </c>
       <c r="F43" t="n">
-        <v>411.2214559580114</v>
+        <v>411.2214559580108</v>
       </c>
       <c r="G43" t="n">
-        <v>268.5553036345476</v>
+        <v>268.555303634547</v>
       </c>
       <c r="H43" t="n">
         <v>151.373419438402</v>
       </c>
       <c r="I43" t="n">
-        <v>93.81666304797187</v>
+        <v>93.81666304797189</v>
       </c>
       <c r="J43" t="n">
         <v>198.094482495415</v>
@@ -7582,37 +7582,37 @@
         <v>1785.769117656414</v>
       </c>
       <c r="O43" t="n">
-        <v>2179.340199382519</v>
+        <v>2179.340199382518</v>
       </c>
       <c r="P43" t="n">
-        <v>2496.057455973197</v>
+        <v>2496.057455973196</v>
       </c>
       <c r="Q43" t="n">
         <v>2639.297491717215</v>
       </c>
       <c r="R43" t="n">
-        <v>2596.781734931274</v>
+        <v>2596.781734931273</v>
       </c>
       <c r="S43" t="n">
         <v>2438.456847547834</v>
       </c>
       <c r="T43" t="n">
-        <v>2243.385329532432</v>
+        <v>2243.385329532431</v>
       </c>
       <c r="U43" t="n">
-        <v>1978.840049838286</v>
+        <v>1978.840049838285</v>
       </c>
       <c r="V43" t="n">
         <v>1748.685508594055</v>
       </c>
       <c r="W43" t="n">
-        <v>1483.798285518751</v>
+        <v>1483.79828551875</v>
       </c>
       <c r="X43" t="n">
-        <v>1280.33868158239</v>
+        <v>1280.338681582389</v>
       </c>
       <c r="Y43" t="n">
-        <v>1084.076049400516</v>
+        <v>1084.076049400515</v>
       </c>
     </row>
     <row r="44">
@@ -7622,19 +7622,19 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>2317.776026551874</v>
+        <v>2317.776026551875</v>
       </c>
       <c r="C44" t="n">
-        <v>1948.813509611462</v>
+        <v>1948.813509611463</v>
       </c>
       <c r="D44" t="n">
-        <v>1590.547811004712</v>
+        <v>1590.547811004713</v>
       </c>
       <c r="E44" t="n">
-        <v>1204.759558406468</v>
+        <v>1204.759558406469</v>
       </c>
       <c r="F44" t="n">
-        <v>793.7736536168609</v>
+        <v>793.7736536168611</v>
       </c>
       <c r="G44" t="n">
         <v>379.8308874362686</v>
@@ -7643,13 +7643,13 @@
         <v>93.81666304797187</v>
       </c>
       <c r="I44" t="n">
-        <v>95.34095638192595</v>
+        <v>95.34095638192616</v>
       </c>
       <c r="J44" t="n">
-        <v>378.1925803111715</v>
+        <v>378.1925803111717</v>
       </c>
       <c r="K44" t="n">
-        <v>852.8523611075807</v>
+        <v>852.8523611075809</v>
       </c>
       <c r="L44" t="n">
         <v>1478.611553332387</v>
@@ -7679,19 +7679,19 @@
         <v>4405.252601474784</v>
       </c>
       <c r="U44" t="n">
-        <v>4151.812499466572</v>
+        <v>4151.812499466573</v>
       </c>
       <c r="V44" t="n">
-        <v>3820.749612123001</v>
+        <v>3820.749612123002</v>
       </c>
       <c r="W44" t="n">
-        <v>3467.980956852887</v>
+        <v>3467.980956852888</v>
       </c>
       <c r="X44" t="n">
-        <v>3094.515198591807</v>
+        <v>3094.515198591808</v>
       </c>
       <c r="Y44" t="n">
-        <v>2704.375866615996</v>
+        <v>2704.375866615997</v>
       </c>
     </row>
     <row r="45">
@@ -7734,19 +7734,19 @@
         <v>1074.481071167373</v>
       </c>
       <c r="M45" t="n">
-        <v>1231.938859683105</v>
+        <v>1671.859558793925</v>
       </c>
       <c r="N45" t="n">
-        <v>1859.536823237711</v>
+        <v>2299.457522348532</v>
       </c>
       <c r="O45" t="n">
-        <v>1859.536823237711</v>
+        <v>2553.061288060775</v>
       </c>
       <c r="P45" t="n">
-        <v>2283.159972732779</v>
+        <v>2553.061288060775</v>
       </c>
       <c r="Q45" t="n">
-        <v>2516.421633107662</v>
+        <v>2553.061288060775</v>
       </c>
       <c r="R45" t="n">
         <v>2553.061288060775</v>
@@ -7780,22 +7780,22 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>926.957531531932</v>
+        <v>926.9575315319327</v>
       </c>
       <c r="C46" t="n">
-        <v>782.5512955656814</v>
+        <v>782.551295565682</v>
       </c>
       <c r="D46" t="n">
-        <v>656.9646031150019</v>
+        <v>656.9646031150025</v>
       </c>
       <c r="E46" t="n">
-        <v>533.581456494265</v>
+        <v>533.5814564942657</v>
       </c>
       <c r="F46" t="n">
-        <v>411.2214559580109</v>
+        <v>411.2214559580116</v>
       </c>
       <c r="G46" t="n">
-        <v>268.5553036345477</v>
+        <v>268.5553036345476</v>
       </c>
       <c r="H46" t="n">
         <v>151.373419438402</v>
@@ -7807,10 +7807,10 @@
         <v>198.094482495415</v>
       </c>
       <c r="K46" t="n">
-        <v>483.8255460380728</v>
+        <v>483.825546038073</v>
       </c>
       <c r="L46" t="n">
-        <v>898.2659412311323</v>
+        <v>898.2659412311324</v>
       </c>
       <c r="M46" t="n">
         <v>1344.317444979286</v>
@@ -7828,16 +7828,16 @@
         <v>2639.297491717215</v>
       </c>
       <c r="R46" t="n">
-        <v>2596.781734931273</v>
+        <v>2596.781734931274</v>
       </c>
       <c r="S46" t="n">
-        <v>2438.456847547834</v>
+        <v>2438.456847547835</v>
       </c>
       <c r="T46" t="n">
         <v>2243.385329532432</v>
       </c>
       <c r="U46" t="n">
-        <v>1978.840049838285</v>
+        <v>1978.840049838286</v>
       </c>
       <c r="V46" t="n">
         <v>1748.685508594055</v>
@@ -7846,10 +7846,10 @@
         <v>1483.798285518751</v>
       </c>
       <c r="X46" t="n">
-        <v>1280.338681582389</v>
+        <v>1280.33868158239</v>
       </c>
       <c r="Y46" t="n">
-        <v>1084.076049400515</v>
+        <v>1084.076049400516</v>
       </c>
     </row>
   </sheetData>
@@ -7976,10 +7976,10 @@
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>169.0966151720738</v>
+        <v>17.30226975545301</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>324.1454125711647</v>
       </c>
       <c r="L2" t="n">
         <v>417.6612145504504</v>
@@ -7991,13 +7991,13 @@
         <v>437.3469244119842</v>
       </c>
       <c r="O2" t="n">
-        <v>173.5591527021829</v>
+        <v>380.8001812627454</v>
       </c>
       <c r="P2" t="n">
-        <v>321.7987081714826</v>
+        <v>140.554421195139</v>
       </c>
       <c r="Q2" t="n">
-        <v>212.3149906599047</v>
+        <v>13.96718192114221</v>
       </c>
       <c r="R2" t="n">
         <v>65.71641987298243</v>
@@ -8055,10 +8055,10 @@
         <v>10.12574714858493</v>
       </c>
       <c r="J3" t="n">
-        <v>126.0910353404088</v>
+        <v>29.31303955311817</v>
       </c>
       <c r="K3" t="n">
-        <v>264.4652370125786</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
         <v>370.8403453034592</v>
@@ -8073,10 +8073,10 @@
         <v>393.8623192767295</v>
       </c>
       <c r="P3" t="n">
-        <v>0.3359151875221542</v>
+        <v>318.4627686399372</v>
       </c>
       <c r="Q3" t="n">
-        <v>8.216508622360777</v>
+        <v>51.33288796981488</v>
       </c>
       <c r="R3" t="n">
         <v>45.52166981132082</v>
@@ -8216,10 +8216,10 @@
         <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>69.4274210713894</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>417.6612145504504</v>
       </c>
       <c r="M5" t="n">
         <v>449.5135334928325</v>
@@ -8228,10 +8228,10 @@
         <v>437.3469244119842</v>
       </c>
       <c r="O5" t="n">
-        <v>380.8001812627454</v>
+        <v>354.365095955167</v>
       </c>
       <c r="P5" t="n">
-        <v>321.7987081714826</v>
+        <v>0</v>
       </c>
       <c r="Q5" t="n">
         <v>0</v>
@@ -8535,19 +8535,19 @@
         <v>264.4652370125786</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>370.8403453034592</v>
       </c>
       <c r="M9" t="n">
-        <v>465.7050637499999</v>
+        <v>48.10560617263505</v>
       </c>
       <c r="N9" t="n">
-        <v>271.7036563660316</v>
+        <v>0</v>
       </c>
       <c r="O9" t="n">
         <v>393.8623192767295</v>
       </c>
       <c r="P9" t="n">
-        <v>0</v>
+        <v>318.4627686399372</v>
       </c>
       <c r="Q9" t="n">
         <v>210.0772877358491</v>
@@ -8696,7 +8696,7 @@
         <v>0</v>
       </c>
       <c r="M11" t="n">
-        <v>0</v>
+        <v>4.547473508864641e-13</v>
       </c>
       <c r="N11" t="n">
         <v>0</v>
@@ -9422,7 +9422,7 @@
         <v>0</v>
       </c>
       <c r="R20" t="n">
-        <v>0</v>
+        <v>4.263256414560601e-13</v>
       </c>
       <c r="S20" t="n">
         <v>0</v>
@@ -9659,7 +9659,7 @@
         <v>0</v>
       </c>
       <c r="R23" t="n">
-        <v>0</v>
+        <v>4.263256414560601e-13</v>
       </c>
       <c r="S23" t="n">
         <v>0</v>
@@ -22556,13 +22556,13 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>406.8760457417114</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>300.072593804393</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -22610,10 +22610,10 @@
         <v>349.240968717413</v>
       </c>
       <c r="X2" t="n">
-        <v>0</v>
+        <v>369.731100678469</v>
       </c>
       <c r="Y2" t="n">
-        <v>0</v>
+        <v>243.8346287659498</v>
       </c>
     </row>
     <row r="3">
@@ -22765,13 +22765,13 @@
         <v>0</v>
       </c>
       <c r="W4" t="n">
-        <v>181.3867393988975</v>
+        <v>272.522071217395</v>
       </c>
       <c r="X4" t="n">
         <v>0</v>
       </c>
       <c r="Y4" t="n">
-        <v>0</v>
+        <v>218.5846533520948</v>
       </c>
     </row>
     <row r="5">
@@ -23315,7 +23315,7 @@
         <v>0</v>
       </c>
       <c r="V11" t="n">
-        <v>1.193711796076968e-12</v>
+        <v>0</v>
       </c>
       <c r="W11" t="n">
         <v>0</v>
@@ -23419,7 +23419,7 @@
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>148.6154730182124</v>
+        <v>0</v>
       </c>
       <c r="E13" t="n">
         <v>146.4339626465692</v>
@@ -23428,7 +23428,7 @@
         <v>145.4210480229312</v>
       </c>
       <c r="G13" t="n">
-        <v>138.4949402405077</v>
+        <v>165.5241382922688</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -23476,7 +23476,7 @@
         <v>0</v>
       </c>
       <c r="W13" t="n">
-        <v>0</v>
+        <v>121.5862749664512</v>
       </c>
       <c r="X13" t="n">
         <v>0</v>
@@ -23656,10 +23656,10 @@
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>148.6154730182124</v>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>146.4339626465692</v>
       </c>
       <c r="F16" t="n">
         <v>145.4210480229312</v>
@@ -23701,10 +23701,10 @@
         <v>0</v>
       </c>
       <c r="S16" t="n">
-        <v>181.0262860016446</v>
+        <v>0</v>
       </c>
       <c r="T16" t="n">
-        <v>0</v>
+        <v>138.4949402405078</v>
       </c>
       <c r="U16" t="n">
         <v>0</v>
@@ -23716,10 +23716,10 @@
         <v>0</v>
       </c>
       <c r="X16" t="n">
-        <v>33.93343655154945</v>
+        <v>0</v>
       </c>
       <c r="Y16" t="n">
-        <v>218.5846533520948</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -23899,16 +23899,16 @@
         <v>146.4339626465692</v>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>145.4210480229312</v>
       </c>
       <c r="G19" t="n">
         <v>0</v>
       </c>
       <c r="H19" t="n">
-        <v>140.2947128462239</v>
+        <v>0</v>
       </c>
       <c r="I19" t="n">
-        <v>77.2460287070935</v>
+        <v>81.26583631856553</v>
       </c>
       <c r="J19" t="n">
         <v>0</v>
@@ -23935,7 +23935,7 @@
         <v>0</v>
       </c>
       <c r="R19" t="n">
-        <v>66.37524671012169</v>
+        <v>0</v>
       </c>
       <c r="S19" t="n">
         <v>0</v>
@@ -23950,7 +23950,7 @@
         <v>0</v>
       </c>
       <c r="W19" t="n">
-        <v>0</v>
+        <v>57.22910392194231</v>
       </c>
       <c r="X19" t="n">
         <v>0</v>
@@ -24139,7 +24139,7 @@
         <v>145.4210480229312</v>
       </c>
       <c r="G22" t="n">
-        <v>57.2291039219422</v>
+        <v>57.22910392194223</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
@@ -24370,16 +24370,16 @@
         <v>148.6154730182124</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>146.4339626465692</v>
       </c>
       <c r="F25" t="n">
         <v>145.4210480229312</v>
       </c>
       <c r="G25" t="n">
-        <v>63.36835372228749</v>
+        <v>57.22910392194223</v>
       </c>
       <c r="H25" t="n">
-        <v>140.2947128462239</v>
+        <v>0</v>
       </c>
       <c r="I25" t="n">
         <v>81.26583631856553</v>
@@ -26311,49 +26311,49 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>32460.91116143664</v>
+        <v>32460.91116143662</v>
       </c>
       <c r="C2" t="n">
         <v>41052.08849321417</v>
       </c>
       <c r="D2" t="n">
+        <v>41052.08849321416</v>
+      </c>
+      <c r="E2" t="n">
+        <v>40357.3299845003</v>
+      </c>
+      <c r="F2" t="n">
+        <v>40357.3299845003</v>
+      </c>
+      <c r="G2" t="n">
+        <v>40357.3299845003</v>
+      </c>
+      <c r="H2" t="n">
+        <v>40357.32998450031</v>
+      </c>
+      <c r="I2" t="n">
+        <v>40357.32998450032</v>
+      </c>
+      <c r="J2" t="n">
+        <v>41052.08849321418</v>
+      </c>
+      <c r="K2" t="n">
         <v>41052.08849321417</v>
       </c>
-      <c r="E2" t="n">
-        <v>40357.32998450031</v>
-      </c>
-      <c r="F2" t="n">
-        <v>40357.32998450031</v>
-      </c>
-      <c r="G2" t="n">
-        <v>40357.32998450031</v>
-      </c>
-      <c r="H2" t="n">
-        <v>40357.32998450028</v>
-      </c>
-      <c r="I2" t="n">
-        <v>40357.3299845003</v>
-      </c>
-      <c r="J2" t="n">
-        <v>41052.0884932142</v>
-      </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>41052.08849321419</v>
       </c>
-      <c r="L2" t="n">
-        <v>41052.08849321418</v>
-      </c>
       <c r="M2" t="n">
-        <v>41052.08849321416</v>
+        <v>41052.08849321419</v>
       </c>
       <c r="N2" t="n">
-        <v>41052.08849321416</v>
+        <v>41052.08849321419</v>
       </c>
       <c r="O2" t="n">
         <v>41052.08849321419</v>
       </c>
       <c r="P2" t="n">
-        <v>41052.08849321419</v>
+        <v>41052.08849321416</v>
       </c>
     </row>
     <row r="3">
@@ -26381,13 +26381,13 @@
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>3.126388037344441e-11</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>191788.7103939126</v>
+        <v>191788.7103939125</v>
       </c>
       <c r="K3" t="n">
         <v>0</v>
@@ -26396,13 +26396,13 @@
         <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>128077.5968157138</v>
+        <v>128077.5968157137</v>
       </c>
       <c r="N3" t="n">
         <v>0</v>
       </c>
       <c r="O3" t="n">
-        <v>19427.71799363184</v>
+        <v>19427.71799363177</v>
       </c>
       <c r="P3" t="n">
         <v>0</v>
@@ -26424,40 +26424,40 @@
         <v>189891.8124216188</v>
       </c>
       <c r="E4" t="n">
-        <v>6897.424496707359</v>
+        <v>6897.424496707369</v>
       </c>
       <c r="F4" t="n">
         <v>6897.424496707359</v>
       </c>
       <c r="G4" t="n">
-        <v>6897.424496707415</v>
+        <v>6897.424496707359</v>
       </c>
       <c r="H4" t="n">
-        <v>6897.424496707401</v>
+        <v>6897.424496707369</v>
       </c>
       <c r="I4" t="n">
-        <v>6897.424496707403</v>
+        <v>6897.424496707392</v>
       </c>
       <c r="J4" t="n">
-        <v>14888.2837598009</v>
+        <v>14888.28375980089</v>
       </c>
       <c r="K4" t="n">
         <v>14888.28375980089</v>
       </c>
       <c r="L4" t="n">
-        <v>14888.2837598009</v>
+        <v>14888.28375980084</v>
       </c>
       <c r="M4" t="n">
+        <v>14888.28375980087</v>
+      </c>
+      <c r="N4" t="n">
         <v>14888.28375980083</v>
-      </c>
-      <c r="N4" t="n">
-        <v>14888.28375980082</v>
       </c>
       <c r="O4" t="n">
         <v>14888.28375980083</v>
       </c>
       <c r="P4" t="n">
-        <v>14888.28375980082</v>
+        <v>14888.28375980084</v>
       </c>
     </row>
     <row r="5">
@@ -26519,49 +26519,49 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-847796.3310365431</v>
+        <v>-848225.8899031321</v>
       </c>
       <c r="C6" t="n">
-        <v>-338877.0299277977</v>
+        <v>-338877.0299277976</v>
       </c>
       <c r="D6" t="n">
         <v>-235457.8017658803</v>
       </c>
       <c r="E6" t="n">
-        <v>-843350.9716126986</v>
+        <v>-843385.7095381343</v>
       </c>
       <c r="F6" t="n">
-        <v>-67662.62433611415</v>
+        <v>-67697.36226154988</v>
       </c>
       <c r="G6" t="n">
-        <v>-67662.6243361142</v>
+        <v>-67697.36226154988</v>
       </c>
       <c r="H6" t="n">
-        <v>-67662.62433611421</v>
+        <v>-67697.3622615499</v>
       </c>
       <c r="I6" t="n">
-        <v>-67662.62433611421</v>
+        <v>-67697.36226154988</v>
       </c>
       <c r="J6" t="n">
-        <v>-268789.0215144147</v>
+        <v>-268789.0215144146</v>
       </c>
       <c r="K6" t="n">
         <v>-77000.3111205021</v>
       </c>
       <c r="L6" t="n">
-        <v>-77000.31112050211</v>
+        <v>-77000.31112050205</v>
       </c>
       <c r="M6" t="n">
         <v>-205077.9079362158</v>
       </c>
       <c r="N6" t="n">
-        <v>-77000.31112050201</v>
+        <v>-77000.31112050204</v>
       </c>
       <c r="O6" t="n">
-        <v>-96428.02911413387</v>
+        <v>-96428.02911413381</v>
       </c>
       <c r="P6" t="n">
-        <v>-77000.31112050203</v>
+        <v>-77000.31112050208</v>
       </c>
     </row>
   </sheetData>
@@ -26701,10 +26701,10 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>3.907985046680551e-14</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>3.907985046680551e-14</v>
       </c>
       <c r="J2" t="n">
         <v>24.28464749203975</v>
@@ -26716,10 +26716,10 @@
         <v>24.28464749203975</v>
       </c>
       <c r="M2" t="n">
+        <v>24.28464749203971</v>
+      </c>
+      <c r="N2" t="n">
         <v>24.28464749203973</v>
-      </c>
-      <c r="N2" t="n">
-        <v>24.28464749203968</v>
       </c>
       <c r="O2" t="n">
         <v>24.28464749203973</v>
@@ -26923,13 +26923,13 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>3.907985046680551e-14</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>24.28464749203975</v>
+        <v>24.28464749203971</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
@@ -26941,10 +26941,10 @@
         <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>-5.329070518200751e-14</v>
+        <v>0</v>
       </c>
       <c r="O2" t="n">
-        <v>24.2846474920398</v>
+        <v>24.28464749203971</v>
       </c>
       <c r="P2" t="n">
         <v>0</v>
@@ -27018,31 +27018,31 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
+        <v>513.9467938544877</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>658.7614942451604</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
         <v>513.9467938544875</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>658.7614942451606</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" t="n">
-        <v>513.9467938544877</v>
       </c>
       <c r="N4" t="n">
         <v>0</v>
@@ -27160,13 +27160,13 @@
         <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>3.907985046680551e-14</v>
       </c>
       <c r="N2" t="n">
         <v>0</v>
       </c>
       <c r="O2" t="n">
-        <v>24.28464749203975</v>
+        <v>24.28464749203971</v>
       </c>
       <c r="P2" t="n">
         <v>0</v>
@@ -27264,7 +27264,7 @@
         <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>513.9467938544875</v>
+        <v>513.9467938544877</v>
       </c>
       <c r="N4" t="n">
         <v>0</v>
@@ -27385,7 +27385,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>192.8063411820582</v>
+        <v>286.1892512837439</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -27467,7 +27467,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>31.71990606559979</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -27476,7 +27476,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>31.7199060655997</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
@@ -27537,7 +27537,7 @@
         <v>179.8319801819373</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>167.2468210986278</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -27588,13 +27588,13 @@
         <v>208.9350332964224</v>
       </c>
       <c r="T4" t="n">
-        <v>224.2479705299724</v>
+        <v>0</v>
       </c>
       <c r="U4" t="n">
-        <v>286.2718257109806</v>
+        <v>0</v>
       </c>
       <c r="V4" t="n">
-        <v>0</v>
+        <v>252.137643323828</v>
       </c>
       <c r="W4" t="n">
         <v>0</v>
@@ -27603,7 +27603,7 @@
         <v>225.7096553890372</v>
       </c>
       <c r="Y4" t="n">
-        <v>218.5846533520948</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -27625,10 +27625,10 @@
         <v>381.9303700722618</v>
       </c>
       <c r="F5" t="n">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -27664,25 +27664,25 @@
         <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>0</v>
+        <v>154.6528871281402</v>
       </c>
       <c r="T5" t="n">
-        <v>0</v>
+        <v>212.651863114966</v>
       </c>
       <c r="U5" t="n">
-        <v>0</v>
+        <v>23.72204591705858</v>
       </c>
       <c r="V5" t="n">
-        <v>327.7522584701349</v>
+        <v>0</v>
       </c>
       <c r="W5" t="n">
         <v>349.240968717413</v>
       </c>
       <c r="X5" t="n">
-        <v>19.24357702455217</v>
+        <v>369.731100678469</v>
       </c>
       <c r="Y5" t="n">
-        <v>0</v>
+        <v>386.2379386560536</v>
       </c>
     </row>
     <row r="6">
@@ -27780,10 +27780,10 @@
         <v>148.6154730182124</v>
       </c>
       <c r="E7" t="n">
-        <v>146.4339626465692</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>145.4210480229312</v>
+        <v>66.28997307420522</v>
       </c>
       <c r="G7" t="n">
         <v>166.9207765545704</v>
@@ -27795,7 +27795,7 @@
         <v>123.266557879417</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>17.69584188176898</v>
       </c>
       <c r="K7" t="n">
         <v>0</v>
@@ -27828,10 +27828,10 @@
         <v>223.3729047207587</v>
       </c>
       <c r="U7" t="n">
-        <v>44.8384689728376</v>
+        <v>286.260654658097</v>
       </c>
       <c r="V7" t="n">
-        <v>252.137643323828</v>
+        <v>0</v>
       </c>
       <c r="W7" t="n">
         <v>0</v>
@@ -27840,7 +27840,7 @@
         <v>0</v>
       </c>
       <c r="Y7" t="n">
-        <v>0</v>
+        <v>218.5846533520948</v>
       </c>
     </row>
     <row r="8">
@@ -27850,28 +27850,28 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>382.7338416634806</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>354.683041620683</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>381.9303700722618</v>
       </c>
       <c r="F8" t="n">
         <v>400</v>
       </c>
       <c r="G8" t="n">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>171.1296183765503</v>
+        <v>268.1411270996346</v>
       </c>
       <c r="I8" t="n">
-        <v>118.4960408938903</v>
+        <v>0</v>
       </c>
       <c r="J8" t="n">
         <v>0</v>
@@ -27901,10 +27901,10 @@
         <v>0</v>
       </c>
       <c r="S8" t="n">
-        <v>154.6528871281402</v>
+        <v>0</v>
       </c>
       <c r="T8" t="n">
-        <v>0</v>
+        <v>212.651863114966</v>
       </c>
       <c r="U8" t="n">
         <v>251.1547862223006</v>
@@ -27913,10 +27913,10 @@
         <v>0</v>
       </c>
       <c r="W8" t="n">
-        <v>0</v>
+        <v>349.240968717413</v>
       </c>
       <c r="X8" t="n">
-        <v>0</v>
+        <v>369.731100678469</v>
       </c>
       <c r="Y8" t="n">
         <v>0</v>
@@ -28008,7 +28008,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>179.8319801819373</v>
       </c>
       <c r="C10" t="n">
         <v>167.2468210986278</v>
@@ -28020,19 +28020,19 @@
         <v>146.4339626465692</v>
       </c>
       <c r="F10" t="n">
-        <v>145.4210480229312</v>
+        <v>92.70990682746606</v>
       </c>
       <c r="G10" t="n">
-        <v>166.9207765545704</v>
+        <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>152.7120966692326</v>
+        <v>0</v>
       </c>
       <c r="I10" t="n">
         <v>123.266557879417</v>
       </c>
       <c r="J10" t="n">
-        <v>17.69584188176898</v>
+        <v>0</v>
       </c>
       <c r="K10" t="n">
         <v>0</v>
@@ -28059,7 +28059,7 @@
         <v>0</v>
       </c>
       <c r="S10" t="n">
-        <v>2.283007817961163</v>
+        <v>205.3658819001186</v>
       </c>
       <c r="T10" t="n">
         <v>223.3729047207587</v>
@@ -28074,10 +28074,10 @@
         <v>286.522998336591</v>
       </c>
       <c r="X10" t="n">
-        <v>0</v>
+        <v>225.7096553890372</v>
       </c>
       <c r="Y10" t="n">
-        <v>218.5846533520948</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -28576,7 +28576,7 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>1.4210854715202e-12</v>
+        <v>0</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
@@ -28849,7 +28849,7 @@
         <v>0</v>
       </c>
       <c r="S20" t="n">
-        <v>9.094947017729282e-13</v>
+        <v>0</v>
       </c>
       <c r="T20" t="n">
         <v>0</v>
@@ -29053,7 +29053,7 @@
         <v>0</v>
       </c>
       <c r="H23" t="n">
-        <v>0</v>
+        <v>5.115907697472721e-13</v>
       </c>
       <c r="I23" t="n">
         <v>0</v>
@@ -29092,7 +29092,7 @@
         <v>0</v>
       </c>
       <c r="U23" t="n">
-        <v>1.13686837721616e-12</v>
+        <v>0</v>
       </c>
       <c r="V23" t="n">
         <v>0</v>
@@ -29272,7 +29272,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0</v>
+        <v>1.193711796076968e-12</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
@@ -29284,7 +29284,7 @@
         <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>1.364242052659392e-12</v>
+        <v>0</v>
       </c>
       <c r="G26" t="n">
         <v>0</v>
@@ -29761,7 +29761,7 @@
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>1.4210854715202e-12</v>
+        <v>0</v>
       </c>
       <c r="H32" t="n">
         <v>0</v>
@@ -30040,7 +30040,7 @@
         <v>0</v>
       </c>
       <c r="U35" t="n">
-        <v>0</v>
+        <v>1.13686837721616e-12</v>
       </c>
       <c r="V35" t="n">
         <v>0</v>
@@ -30141,76 +30141,76 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>24.28464749203973</v>
+        <v>24.28464749203971</v>
       </c>
       <c r="C37" t="n">
-        <v>24.28464749203973</v>
+        <v>24.28464749203971</v>
       </c>
       <c r="D37" t="n">
-        <v>24.28464749203973</v>
+        <v>24.28464749203971</v>
       </c>
       <c r="E37" t="n">
-        <v>24.28464749203973</v>
+        <v>24.28464749203971</v>
       </c>
       <c r="F37" t="n">
-        <v>24.28464749203973</v>
+        <v>24.28464749203971</v>
       </c>
       <c r="G37" t="n">
-        <v>24.28464749203973</v>
+        <v>24.28464749203971</v>
       </c>
       <c r="H37" t="n">
-        <v>24.28464749203973</v>
+        <v>24.28464749203971</v>
       </c>
       <c r="I37" t="n">
-        <v>24.28464749203973</v>
+        <v>24.28464749203971</v>
       </c>
       <c r="J37" t="n">
-        <v>24.28464749203973</v>
+        <v>24.28464749203971</v>
       </c>
       <c r="K37" t="n">
-        <v>24.28464749203973</v>
+        <v>24.28464749203971</v>
       </c>
       <c r="L37" t="n">
-        <v>24.28464749203973</v>
+        <v>24.28464749203971</v>
       </c>
       <c r="M37" t="n">
-        <v>24.28464749203973</v>
+        <v>24.28464749203971</v>
       </c>
       <c r="N37" t="n">
-        <v>24.28464749203973</v>
+        <v>24.28464749203971</v>
       </c>
       <c r="O37" t="n">
-        <v>24.28464749203973</v>
+        <v>24.28464749203971</v>
       </c>
       <c r="P37" t="n">
-        <v>24.28464749203973</v>
+        <v>24.28464749203971</v>
       </c>
       <c r="Q37" t="n">
-        <v>24.28464749203973</v>
+        <v>24.28464749203971</v>
       </c>
       <c r="R37" t="n">
-        <v>24.28464749203973</v>
+        <v>24.28464749203971</v>
       </c>
       <c r="S37" t="n">
-        <v>24.28464749203973</v>
+        <v>24.28464749203971</v>
       </c>
       <c r="T37" t="n">
-        <v>24.28464749203973</v>
+        <v>24.28464749203971</v>
       </c>
       <c r="U37" t="n">
-        <v>24.28464749203973</v>
+        <v>24.28464749203971</v>
       </c>
       <c r="V37" t="n">
-        <v>24.28464749203973</v>
+        <v>24.28464749203971</v>
       </c>
       <c r="W37" t="n">
-        <v>24.28464749203973</v>
+        <v>24.28464749203971</v>
       </c>
       <c r="X37" t="n">
-        <v>24.28464749203973</v>
+        <v>24.28464749203971</v>
       </c>
       <c r="Y37" t="n">
-        <v>24.28464749203973</v>
+        <v>24.28464749203971</v>
       </c>
     </row>
     <row r="38">
@@ -30378,76 +30378,76 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>24.28464749203968</v>
+        <v>24.28464749203973</v>
       </c>
       <c r="C40" t="n">
-        <v>24.28464749203968</v>
+        <v>24.28464749203973</v>
       </c>
       <c r="D40" t="n">
-        <v>24.28464749203968</v>
+        <v>24.28464749203973</v>
       </c>
       <c r="E40" t="n">
-        <v>24.28464749203968</v>
+        <v>24.28464749203973</v>
       </c>
       <c r="F40" t="n">
-        <v>24.28464749203968</v>
+        <v>24.28464749203973</v>
       </c>
       <c r="G40" t="n">
-        <v>24.28464749203968</v>
+        <v>24.28464749203973</v>
       </c>
       <c r="H40" t="n">
-        <v>24.28464749203968</v>
+        <v>24.28464749203973</v>
       </c>
       <c r="I40" t="n">
-        <v>24.28464749203968</v>
+        <v>24.28464749203973</v>
       </c>
       <c r="J40" t="n">
-        <v>24.28464749203968</v>
+        <v>24.28464749203973</v>
       </c>
       <c r="K40" t="n">
-        <v>24.28464749203968</v>
+        <v>24.28464749203973</v>
       </c>
       <c r="L40" t="n">
-        <v>24.28464749203968</v>
+        <v>24.28464749203973</v>
       </c>
       <c r="M40" t="n">
-        <v>24.28464749203968</v>
+        <v>24.28464749203973</v>
       </c>
       <c r="N40" t="n">
-        <v>24.28464749203968</v>
+        <v>24.28464749203973</v>
       </c>
       <c r="O40" t="n">
-        <v>24.28464749203968</v>
+        <v>24.28464749203973</v>
       </c>
       <c r="P40" t="n">
-        <v>24.28464749203968</v>
+        <v>24.28464749203973</v>
       </c>
       <c r="Q40" t="n">
-        <v>24.28464749203968</v>
+        <v>24.28464749203973</v>
       </c>
       <c r="R40" t="n">
-        <v>24.28464749203968</v>
+        <v>24.28464749203973</v>
       </c>
       <c r="S40" t="n">
-        <v>24.28464749203968</v>
+        <v>24.28464749203973</v>
       </c>
       <c r="T40" t="n">
-        <v>24.28464749203968</v>
+        <v>24.28464749203973</v>
       </c>
       <c r="U40" t="n">
-        <v>24.28464749203968</v>
+        <v>24.28464749203973</v>
       </c>
       <c r="V40" t="n">
-        <v>24.28464749203968</v>
+        <v>24.28464749203973</v>
       </c>
       <c r="W40" t="n">
-        <v>24.28464749203968</v>
+        <v>24.28464749203973</v>
       </c>
       <c r="X40" t="n">
-        <v>24.28464749203968</v>
+        <v>24.28464749203973</v>
       </c>
       <c r="Y40" t="n">
-        <v>24.28464749203968</v>
+        <v>24.28464749203973</v>
       </c>
     </row>
     <row r="41">
@@ -30697,7 +30697,7 @@
         <v>0</v>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>4.547473508864641e-13</v>
       </c>
       <c r="D44" t="n">
         <v>0</v>
@@ -31835,7 +31835,7 @@
         <v>28.417755205211</v>
       </c>
       <c r="I12" t="n">
-        <v>99.52238</v>
+        <v>101.3076196007749</v>
       </c>
       <c r="J12" t="n">
         <v>277.9958514420755</v>
@@ -31850,16 +31850,16 @@
         <v>745.5466476862121</v>
       </c>
       <c r="N12" t="n">
-        <v>131.3417120833333</v>
+        <v>765.2790490071785</v>
       </c>
       <c r="O12" t="n">
-        <v>370.9642309107746</v>
+        <v>398.7616643558013</v>
       </c>
       <c r="P12" t="n">
-        <v>561.8765786214698</v>
+        <v>133.9744074143302</v>
       </c>
       <c r="Q12" t="n">
-        <v>375.599612848529</v>
+        <v>139.9817740860215</v>
       </c>
       <c r="R12" t="n">
         <v>145.679503963964</v>
@@ -32072,7 +32072,7 @@
         <v>28.417755205211</v>
       </c>
       <c r="I15" t="n">
-        <v>99.52238</v>
+        <v>101.3076196007749</v>
       </c>
       <c r="J15" t="n">
         <v>277.9958514420755</v>
@@ -32087,16 +32087,16 @@
         <v>745.5466476862121</v>
       </c>
       <c r="N15" t="n">
-        <v>359.7096985496635</v>
+        <v>765.2790490071785</v>
       </c>
       <c r="O15" t="n">
-        <v>142.5962444444444</v>
+        <v>398.7616643558013</v>
       </c>
       <c r="P15" t="n">
-        <v>561.8765786214698</v>
+        <v>133.9744074143302</v>
       </c>
       <c r="Q15" t="n">
-        <v>375.599612848529</v>
+        <v>139.9817740860215</v>
       </c>
       <c r="R15" t="n">
         <v>145.679503963964</v>
@@ -32309,7 +32309,7 @@
         <v>28.417755205211</v>
       </c>
       <c r="I18" t="n">
-        <v>99.52238</v>
+        <v>101.3076196007749</v>
       </c>
       <c r="J18" t="n">
         <v>277.9958514420755</v>
@@ -32324,7 +32324,7 @@
         <v>745.5466476862121</v>
       </c>
       <c r="N18" t="n">
-        <v>322.6999460717714</v>
+        <v>320.9147064709964</v>
       </c>
       <c r="O18" t="n">
         <v>142.5962444444444</v>
@@ -32558,22 +32558,22 @@
         <v>638.8832749473072</v>
       </c>
       <c r="M21" t="n">
-        <v>745.5466476862121</v>
+        <v>573.8098963904297</v>
       </c>
       <c r="N21" t="n">
         <v>765.2790490071785</v>
       </c>
       <c r="O21" t="n">
-        <v>361.7519118779092</v>
+        <v>142.5962444444444</v>
       </c>
       <c r="P21" t="n">
-        <v>133.9744074143302</v>
+        <v>561.8765786214698</v>
       </c>
       <c r="Q21" t="n">
         <v>139.9817740860215</v>
       </c>
       <c r="R21" t="n">
-        <v>182.6892564418561</v>
+        <v>145.679503963964</v>
       </c>
       <c r="S21" t="n">
         <v>54.65449286742438</v>
@@ -32798,16 +32798,16 @@
         <v>745.5466476862121</v>
       </c>
       <c r="N24" t="n">
-        <v>131.3417120833333</v>
+        <v>765.2790490071785</v>
       </c>
       <c r="O24" t="n">
-        <v>369.1789913099997</v>
+        <v>398.7616643558013</v>
       </c>
       <c r="P24" t="n">
-        <v>561.8765786214698</v>
+        <v>133.9744074143302</v>
       </c>
       <c r="Q24" t="n">
-        <v>375.599612848529</v>
+        <v>139.9817740860215</v>
       </c>
       <c r="R24" t="n">
         <v>145.679503963964</v>
@@ -33026,7 +33026,7 @@
         <v>277.9958514420755</v>
       </c>
       <c r="K27" t="n">
-        <v>137.841438974359</v>
+        <v>475.1391886422585</v>
       </c>
       <c r="L27" t="n">
         <v>638.8832749473072</v>
@@ -33038,7 +33038,7 @@
         <v>765.2790490071785</v>
       </c>
       <c r="O27" t="n">
-        <v>699.0496615458086</v>
+        <v>398.7616643558013</v>
       </c>
       <c r="P27" t="n">
         <v>133.9744074143302</v>
@@ -33047,7 +33047,7 @@
         <v>139.9817740860215</v>
       </c>
       <c r="R27" t="n">
-        <v>182.6892564418561</v>
+        <v>145.679503963964</v>
       </c>
       <c r="S27" t="n">
         <v>54.65449286742438</v>
@@ -33266,7 +33266,7 @@
         <v>475.1391886422585</v>
       </c>
       <c r="L30" t="n">
-        <v>337.5641188593844</v>
+        <v>638.8832749473072</v>
       </c>
       <c r="M30" t="n">
         <v>745.5466476862121</v>
@@ -33275,7 +33275,7 @@
         <v>765.2790490071785</v>
       </c>
       <c r="O30" t="n">
-        <v>700.0808204437243</v>
+        <v>398.7616643558013</v>
       </c>
       <c r="P30" t="n">
         <v>133.9744074143302</v>
@@ -34153,7 +34153,7 @@
         <v>593.8732233669223</v>
       </c>
       <c r="R41" t="n">
-        <v>345.4516222043725</v>
+        <v>345.4516222043729</v>
       </c>
       <c r="S41" t="n">
         <v>125.31755462929</v>
@@ -34205,34 +34205,34 @@
         <v>28.417755205211</v>
       </c>
       <c r="I42" t="n">
-        <v>99.52238</v>
+        <v>101.3076196007749</v>
       </c>
       <c r="J42" t="n">
-        <v>126.8376266666667</v>
+        <v>277.9958514420755</v>
       </c>
       <c r="K42" t="n">
-        <v>137.841438974359</v>
+        <v>475.1391886422585</v>
       </c>
       <c r="L42" t="n">
-        <v>138.5543797798742</v>
+        <v>638.8832749473072</v>
       </c>
       <c r="M42" t="n">
-        <v>734.2678383622665</v>
+        <v>745.5466476862121</v>
       </c>
       <c r="N42" t="n">
         <v>765.2790490071785</v>
       </c>
       <c r="O42" t="n">
-        <v>700.0808204437243</v>
+        <v>398.7616643558013</v>
       </c>
       <c r="P42" t="n">
-        <v>561.8765786214698</v>
+        <v>133.9744074143302</v>
       </c>
       <c r="Q42" t="n">
-        <v>375.599612848529</v>
+        <v>139.9817740860215</v>
       </c>
       <c r="R42" t="n">
-        <v>182.6892564418561</v>
+        <v>145.679503963964</v>
       </c>
       <c r="S42" t="n">
         <v>54.65449286742438</v>
@@ -34378,7 +34378,7 @@
         <v>965.6463440175675</v>
       </c>
       <c r="N44" t="n">
-        <v>981.2715114159428</v>
+        <v>981.2715114159425</v>
       </c>
       <c r="O44" t="n">
         <v>926.5868626460027</v>
@@ -34454,22 +34454,22 @@
         <v>638.8832749473072</v>
       </c>
       <c r="M45" t="n">
-        <v>301.1823051500301</v>
+        <v>745.5466476862121</v>
       </c>
       <c r="N45" t="n">
         <v>765.2790490071785</v>
       </c>
       <c r="O45" t="n">
-        <v>142.5962444444444</v>
+        <v>398.7616643558013</v>
       </c>
       <c r="P45" t="n">
-        <v>561.8765786214698</v>
+        <v>133.9744074143302</v>
       </c>
       <c r="Q45" t="n">
-        <v>375.599612848529</v>
+        <v>139.9817740860215</v>
       </c>
       <c r="R45" t="n">
-        <v>182.6892564418561</v>
+        <v>145.679503963964</v>
       </c>
       <c r="S45" t="n">
         <v>54.65449286742438</v>
@@ -34696,10 +34696,10 @@
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>151.7943454166208</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>25.31941131860373</v>
+        <v>349.4648238897685</v>
       </c>
       <c r="L2" t="n">
         <v>486.3466901138895</v>
@@ -34711,13 +34711,13 @@
         <v>552.1767640842847</v>
       </c>
       <c r="O2" t="n">
-        <v>268.5197532578346</v>
+        <v>475.760781818397</v>
       </c>
       <c r="P2" t="n">
-        <v>367.9958879374644</v>
+        <v>186.7516009611207</v>
       </c>
       <c r="Q2" t="n">
-        <v>198.3478087387625</v>
+        <v>0</v>
       </c>
       <c r="R2" t="n">
         <v>0</v>
@@ -34775,10 +34775,10 @@
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>96.77799578729066</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>293.3088509029666</v>
+        <v>28.84361389038801</v>
       </c>
       <c r="L3" t="n">
         <v>456.4145893133914</v>
@@ -34793,10 +34793,10 @@
         <v>496.8635994202181</v>
       </c>
       <c r="P3" t="n">
-        <v>63.47517351525008</v>
+        <v>381.6020269676651</v>
       </c>
       <c r="Q3" t="n">
-        <v>0</v>
+        <v>43.1163793474541</v>
       </c>
       <c r="R3" t="n">
         <v>0</v>
@@ -34936,10 +34936,10 @@
         <v>21.44873736705384</v>
       </c>
       <c r="K5" t="n">
-        <v>152.824546904311</v>
+        <v>83.39712583292157</v>
       </c>
       <c r="L5" t="n">
-        <v>140.7360160012659</v>
+        <v>558.3972305517163</v>
       </c>
       <c r="M5" t="n">
         <v>638.0987989730422</v>
@@ -34948,10 +34948,10 @@
         <v>633.6441091513602</v>
       </c>
       <c r="O5" t="n">
-        <v>552.6880856233105</v>
+        <v>526.2530003157322</v>
       </c>
       <c r="P5" t="n">
-        <v>433.6515619588832</v>
+        <v>111.8528537874005</v>
       </c>
       <c r="Q5" t="n">
         <v>35.33749497130819</v>
@@ -35255,19 +35255,19 @@
         <v>332.7559639452625</v>
       </c>
       <c r="L9" t="n">
-        <v>138.615755571408</v>
+        <v>509.4561008748672</v>
       </c>
       <c r="M9" t="n">
-        <v>647.0155045122269</v>
+        <v>229.4160469348621</v>
       </c>
       <c r="N9" t="n">
-        <v>472.3670317727637</v>
+        <v>200.663375406732</v>
       </c>
       <c r="O9" t="n">
         <v>554.9858674269929</v>
       </c>
       <c r="P9" t="n">
-        <v>109.7875025528271</v>
+        <v>428.2502711927643</v>
       </c>
       <c r="Q9" t="n">
         <v>233.0438950105733</v>
@@ -35416,7 +35416,7 @@
         <v>632.0799921462688</v>
       </c>
       <c r="M11" t="n">
-        <v>735.3001107902948</v>
+        <v>735.3001107902952</v>
       </c>
       <c r="N11" t="n">
         <v>751.8584478193516</v>
@@ -35483,7 +35483,7 @@
         <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>1.785239600774915</v>
       </c>
       <c r="J12" t="n">
         <v>151.1582247754088</v>
@@ -35498,16 +35498,16 @@
         <v>603.4126137641938</v>
       </c>
       <c r="N12" t="n">
-        <v>0</v>
+        <v>633.9373369238452</v>
       </c>
       <c r="O12" t="n">
-        <v>228.3679864663302</v>
+        <v>256.1654199113569</v>
       </c>
       <c r="P12" t="n">
-        <v>427.9021712071395</v>
+        <v>0</v>
       </c>
       <c r="Q12" t="n">
-        <v>235.6178387625075</v>
+        <v>0</v>
       </c>
       <c r="R12" t="n">
         <v>0</v>
@@ -35644,7 +35644,7 @@
         <v>1.539690236317256</v>
       </c>
       <c r="J14" t="n">
-        <v>285.7087110396416</v>
+        <v>285.708711039642</v>
       </c>
       <c r="K14" t="n">
         <v>479.454324036777</v>
@@ -35720,7 +35720,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>1.785239600774915</v>
       </c>
       <c r="J15" t="n">
         <v>151.1582247754088</v>
@@ -35735,16 +35735,16 @@
         <v>603.4126137641938</v>
       </c>
       <c r="N15" t="n">
-        <v>228.3679864663302</v>
+        <v>633.9373369238452</v>
       </c>
       <c r="O15" t="n">
-        <v>0</v>
+        <v>256.1654199113569</v>
       </c>
       <c r="P15" t="n">
-        <v>427.9021712071395</v>
+        <v>0</v>
       </c>
       <c r="Q15" t="n">
-        <v>235.6178387625075</v>
+        <v>0</v>
       </c>
       <c r="R15" t="n">
         <v>0</v>
@@ -35905,7 +35905,7 @@
         <v>371.5675334924728</v>
       </c>
       <c r="R17" t="n">
-        <v>129.8660843902399</v>
+        <v>129.8660843902404</v>
       </c>
       <c r="S17" t="n">
         <v>0</v>
@@ -35957,7 +35957,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>1.785239600774915</v>
       </c>
       <c r="J18" t="n">
         <v>151.1582247754088</v>
@@ -35972,7 +35972,7 @@
         <v>603.4126137641938</v>
       </c>
       <c r="N18" t="n">
-        <v>191.358233988438</v>
+        <v>189.5729943876631</v>
       </c>
       <c r="O18" t="n">
         <v>0</v>
@@ -36142,7 +36142,7 @@
         <v>371.5675334924728</v>
       </c>
       <c r="R20" t="n">
-        <v>129.8660843902404</v>
+        <v>129.8660843902408</v>
       </c>
       <c r="S20" t="n">
         <v>0</v>
@@ -36206,22 +36206,22 @@
         <v>500.328895167433</v>
       </c>
       <c r="M21" t="n">
-        <v>603.4126137641938</v>
+        <v>431.6758624684114</v>
       </c>
       <c r="N21" t="n">
         <v>633.9373369238452</v>
       </c>
       <c r="O21" t="n">
-        <v>219.1556674334648</v>
+        <v>0</v>
       </c>
       <c r="P21" t="n">
-        <v>0</v>
+        <v>427.9021712071395</v>
       </c>
       <c r="Q21" t="n">
         <v>0</v>
       </c>
       <c r="R21" t="n">
-        <v>37.00975247789211</v>
+        <v>0</v>
       </c>
       <c r="S21" t="n">
         <v>0</v>
@@ -36364,7 +36364,7 @@
         <v>632.0799921462688</v>
       </c>
       <c r="M23" t="n">
-        <v>735.3001107902943</v>
+        <v>735.3001107902948</v>
       </c>
       <c r="N23" t="n">
         <v>751.8584478193516</v>
@@ -36379,7 +36379,7 @@
         <v>371.5675334924728</v>
       </c>
       <c r="R23" t="n">
-        <v>129.8660843902404</v>
+        <v>129.8660843902408</v>
       </c>
       <c r="S23" t="n">
         <v>0</v>
@@ -36446,16 +36446,16 @@
         <v>603.4126137641938</v>
       </c>
       <c r="N24" t="n">
-        <v>0</v>
+        <v>633.9373369238452</v>
       </c>
       <c r="O24" t="n">
-        <v>226.5827468655553</v>
+        <v>256.1654199113569</v>
       </c>
       <c r="P24" t="n">
-        <v>427.9021712071395</v>
+        <v>0</v>
       </c>
       <c r="Q24" t="n">
-        <v>235.6178387625075</v>
+        <v>0</v>
       </c>
       <c r="R24" t="n">
         <v>0</v>
@@ -36674,7 +36674,7 @@
         <v>151.1582247754088</v>
       </c>
       <c r="K27" t="n">
-        <v>0</v>
+        <v>337.2977496678996</v>
       </c>
       <c r="L27" t="n">
         <v>500.328895167433</v>
@@ -36686,7 +36686,7 @@
         <v>633.9373369238452</v>
       </c>
       <c r="O27" t="n">
-        <v>556.4534171013642</v>
+        <v>256.1654199113569</v>
       </c>
       <c r="P27" t="n">
         <v>0</v>
@@ -36695,7 +36695,7 @@
         <v>0</v>
       </c>
       <c r="R27" t="n">
-        <v>37.00975247789211</v>
+        <v>0</v>
       </c>
       <c r="S27" t="n">
         <v>0</v>
@@ -36914,7 +36914,7 @@
         <v>337.2977496678996</v>
       </c>
       <c r="L30" t="n">
-        <v>199.0097390795102</v>
+        <v>500.328895167433</v>
       </c>
       <c r="M30" t="n">
         <v>603.4126137641938</v>
@@ -36923,7 +36923,7 @@
         <v>633.9373369238452</v>
       </c>
       <c r="O30" t="n">
-        <v>557.4845759992799</v>
+        <v>256.1654199113569</v>
       </c>
       <c r="P30" t="n">
         <v>0</v>
@@ -37236,7 +37236,7 @@
         <v>450.5570744930849</v>
       </c>
       <c r="N34" t="n">
-        <v>445.9107804819471</v>
+        <v>445.9107804819472</v>
       </c>
       <c r="O34" t="n">
         <v>397.5465471980852</v>
@@ -37482,7 +37482,7 @@
         <v>319.9164207986647</v>
       </c>
       <c r="Q37" t="n">
-        <v>144.6869047919381</v>
+        <v>144.686904791938</v>
       </c>
       <c r="R37" t="n">
         <v>0</v>
@@ -37698,13 +37698,13 @@
         <v>0</v>
       </c>
       <c r="J40" t="n">
-        <v>105.331130754993</v>
+        <v>105.3311307549931</v>
       </c>
       <c r="K40" t="n">
-        <v>288.6172359016746</v>
+        <v>288.6172359016747</v>
       </c>
       <c r="L40" t="n">
-        <v>418.6266618111711</v>
+        <v>418.6266618111712</v>
       </c>
       <c r="M40" t="n">
         <v>450.5570744930848</v>
@@ -37716,10 +37716,10 @@
         <v>397.5465471980851</v>
       </c>
       <c r="P40" t="n">
-        <v>319.9164207986646</v>
+        <v>319.9164207986647</v>
       </c>
       <c r="Q40" t="n">
-        <v>144.686904791938</v>
+        <v>144.6869047919381</v>
       </c>
       <c r="R40" t="n">
         <v>0</v>
@@ -37801,7 +37801,7 @@
         <v>371.5675334924728</v>
       </c>
       <c r="R41" t="n">
-        <v>129.8660843902404</v>
+        <v>129.8660843902408</v>
       </c>
       <c r="S41" t="n">
         <v>0</v>
@@ -37853,34 +37853,34 @@
         <v>0</v>
       </c>
       <c r="I42" t="n">
-        <v>0</v>
+        <v>1.785239600774915</v>
       </c>
       <c r="J42" t="n">
-        <v>0</v>
+        <v>151.1582247754088</v>
       </c>
       <c r="K42" t="n">
-        <v>0</v>
+        <v>337.2977496678996</v>
       </c>
       <c r="L42" t="n">
-        <v>0</v>
+        <v>500.328895167433</v>
       </c>
       <c r="M42" t="n">
-        <v>592.1338044402481</v>
+        <v>603.4126137641938</v>
       </c>
       <c r="N42" t="n">
         <v>633.9373369238452</v>
       </c>
       <c r="O42" t="n">
-        <v>557.4845759992799</v>
+        <v>256.1654199113569</v>
       </c>
       <c r="P42" t="n">
-        <v>427.9021712071395</v>
+        <v>0</v>
       </c>
       <c r="Q42" t="n">
-        <v>235.6178387625075</v>
+        <v>0</v>
       </c>
       <c r="R42" t="n">
-        <v>37.00975247789211</v>
+        <v>0</v>
       </c>
       <c r="S42" t="n">
         <v>0</v>
@@ -38026,7 +38026,7 @@
         <v>735.3001107902948</v>
       </c>
       <c r="N44" t="n">
-        <v>751.8584478193519</v>
+        <v>751.8584478193516</v>
       </c>
       <c r="O44" t="n">
         <v>696.488651224316</v>
@@ -38102,22 +38102,22 @@
         <v>500.328895167433</v>
       </c>
       <c r="M45" t="n">
-        <v>159.0482712280117</v>
+        <v>603.4126137641938</v>
       </c>
       <c r="N45" t="n">
         <v>633.9373369238452</v>
       </c>
       <c r="O45" t="n">
-        <v>0</v>
+        <v>256.1654199113569</v>
       </c>
       <c r="P45" t="n">
-        <v>427.9021712071395</v>
+        <v>0</v>
       </c>
       <c r="Q45" t="n">
-        <v>235.6178387625075</v>
+        <v>0</v>
       </c>
       <c r="R45" t="n">
-        <v>37.00975247789211</v>
+        <v>0</v>
       </c>
       <c r="S45" t="n">
         <v>0</v>

</xml_diff>